<commit_message>
corrected template table data constraint.
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/template.xlsx
+++ b/mosip_master/xlsx/template.xlsx
@@ -4209,9 +4209,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:M464"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A114" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D94" sqref="D94"/>
     </sheetView>
   </sheetViews>
@@ -4315,7 +4316,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:13" hidden="1">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -4357,7 +4358,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:13" hidden="1">
       <c r="A4" t="s">
         <v>27</v>
       </c>
@@ -4441,7 +4442,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:13" hidden="1">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -4483,7 +4484,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:13" hidden="1">
       <c r="A7" t="s">
         <v>27</v>
       </c>
@@ -4566,7 +4567,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:13" hidden="1">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -4607,7 +4608,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="45">
+    <row r="10" spans="1:13" ht="45" hidden="1">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -4648,7 +4649,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:13">
+    <row r="11" spans="1:13" hidden="1">
       <c r="A11" t="s">
         <v>47</v>
       </c>
@@ -4690,7 +4691,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:13">
+    <row r="12" spans="1:13" hidden="1">
       <c r="A12" t="s">
         <v>52</v>
       </c>
@@ -4732,7 +4733,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:13">
+    <row r="13" spans="1:13" hidden="1">
       <c r="A13" t="s">
         <v>56</v>
       </c>
@@ -4774,7 +4775,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:13">
+    <row r="14" spans="1:13" hidden="1">
       <c r="A14" t="s">
         <v>60</v>
       </c>
@@ -4816,7 +4817,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:13">
+    <row r="15" spans="1:13" hidden="1">
       <c r="A15" t="s">
         <v>64</v>
       </c>
@@ -4858,7 +4859,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:13">
+    <row r="16" spans="1:13" hidden="1">
       <c r="A16" t="s">
         <v>68</v>
       </c>
@@ -4900,7 +4901,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:13">
+    <row r="17" spans="1:13" hidden="1">
       <c r="A17" t="s">
         <v>72</v>
       </c>
@@ -4942,7 +4943,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:13">
+    <row r="18" spans="1:13" hidden="1">
       <c r="A18" t="s">
         <v>76</v>
       </c>
@@ -4984,7 +4985,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:13">
+    <row r="19" spans="1:13" hidden="1">
       <c r="A19" t="s">
         <v>47</v>
       </c>
@@ -5026,7 +5027,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:13">
+    <row r="20" spans="1:13" hidden="1">
       <c r="A20" t="s">
         <v>52</v>
       </c>
@@ -5068,7 +5069,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="1:13">
+    <row r="21" spans="1:13" hidden="1">
       <c r="A21" t="s">
         <v>56</v>
       </c>
@@ -5110,7 +5111,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="1:13">
+    <row r="22" spans="1:13" hidden="1">
       <c r="A22" t="s">
         <v>60</v>
       </c>
@@ -5152,7 +5153,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:13">
+    <row r="23" spans="1:13" hidden="1">
       <c r="A23" t="s">
         <v>64</v>
       </c>
@@ -5194,7 +5195,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:13">
+    <row r="24" spans="1:13" hidden="1">
       <c r="A24" t="s">
         <v>68</v>
       </c>
@@ -5236,7 +5237,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:13">
+    <row r="25" spans="1:13" hidden="1">
       <c r="A25" t="s">
         <v>72</v>
       </c>
@@ -5278,7 +5279,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:13">
+    <row r="26" spans="1:13" hidden="1">
       <c r="A26" t="s">
         <v>76</v>
       </c>
@@ -5320,7 +5321,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="27" spans="1:13" ht="45">
+    <row r="27" spans="1:13" ht="45" hidden="1">
       <c r="A27" t="s">
         <v>47</v>
       </c>
@@ -5361,7 +5362,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="28" spans="1:13" ht="45">
+    <row r="28" spans="1:13" ht="45" hidden="1">
       <c r="A28" t="s">
         <v>52</v>
       </c>
@@ -5402,7 +5403,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="29" spans="1:13" ht="45">
+    <row r="29" spans="1:13" ht="45" hidden="1">
       <c r="A29" t="s">
         <v>56</v>
       </c>
@@ -5443,7 +5444,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="30" spans="1:13" ht="45">
+    <row r="30" spans="1:13" ht="45" hidden="1">
       <c r="A30" t="s">
         <v>60</v>
       </c>
@@ -5484,7 +5485,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="31" spans="1:13" ht="30">
+    <row r="31" spans="1:13" ht="30" hidden="1">
       <c r="A31" t="s">
         <v>64</v>
       </c>
@@ -5525,7 +5526,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="32" spans="1:13" ht="30">
+    <row r="32" spans="1:13" ht="30" hidden="1">
       <c r="A32" t="s">
         <v>68</v>
       </c>
@@ -5566,7 +5567,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="33" spans="1:13" ht="45">
+    <row r="33" spans="1:13" ht="45" hidden="1">
       <c r="A33" t="s">
         <v>72</v>
       </c>
@@ -5607,7 +5608,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="34" spans="1:13" ht="45">
+    <row r="34" spans="1:13" ht="45" hidden="1">
       <c r="A34" t="s">
         <v>76</v>
       </c>
@@ -5648,7 +5649,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="35" spans="1:13">
+    <row r="35" spans="1:13" hidden="1">
       <c r="A35" t="s">
         <v>114</v>
       </c>
@@ -5690,7 +5691,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="36" spans="1:13">
+    <row r="36" spans="1:13" hidden="1">
       <c r="A36" t="s">
         <v>119</v>
       </c>
@@ -5732,7 +5733,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="37" spans="1:13">
+    <row r="37" spans="1:13" hidden="1">
       <c r="A37" t="s">
         <v>123</v>
       </c>
@@ -5774,7 +5775,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="38" spans="1:13">
+    <row r="38" spans="1:13" hidden="1">
       <c r="A38" t="s">
         <v>126</v>
       </c>
@@ -5816,7 +5817,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="39" spans="1:13">
+    <row r="39" spans="1:13" hidden="1">
       <c r="A39" t="s">
         <v>130</v>
       </c>
@@ -5858,7 +5859,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="40" spans="1:13">
+    <row r="40" spans="1:13" hidden="1">
       <c r="A40" t="s">
         <v>134</v>
       </c>
@@ -5900,7 +5901,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="41" spans="1:13">
+    <row r="41" spans="1:13" hidden="1">
       <c r="A41" t="s">
         <v>137</v>
       </c>
@@ -5942,7 +5943,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="42" spans="1:13">
+    <row r="42" spans="1:13" hidden="1">
       <c r="A42" t="s">
         <v>141</v>
       </c>
@@ -5984,7 +5985,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="43" spans="1:13">
+    <row r="43" spans="1:13" hidden="1">
       <c r="A43" t="s">
         <v>145</v>
       </c>
@@ -6026,7 +6027,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="44" spans="1:13">
+    <row r="44" spans="1:13" hidden="1">
       <c r="A44" t="s">
         <v>114</v>
       </c>
@@ -6068,7 +6069,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="45" spans="1:13">
+    <row r="45" spans="1:13" hidden="1">
       <c r="A45" t="s">
         <v>119</v>
       </c>
@@ -6110,7 +6111,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="46" spans="1:13">
+    <row r="46" spans="1:13" hidden="1">
       <c r="A46" t="s">
         <v>123</v>
       </c>
@@ -6152,7 +6153,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="47" spans="1:13">
+    <row r="47" spans="1:13" hidden="1">
       <c r="A47" t="s">
         <v>126</v>
       </c>
@@ -6194,7 +6195,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="48" spans="1:13">
+    <row r="48" spans="1:13" hidden="1">
       <c r="A48" t="s">
         <v>130</v>
       </c>
@@ -6236,7 +6237,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="49" spans="1:13">
+    <row r="49" spans="1:13" hidden="1">
       <c r="A49" t="s">
         <v>134</v>
       </c>
@@ -6278,7 +6279,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="50" spans="1:13">
+    <row r="50" spans="1:13" hidden="1">
       <c r="A50" t="s">
         <v>137</v>
       </c>
@@ -6320,7 +6321,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="51" spans="1:13">
+    <row r="51" spans="1:13" hidden="1">
       <c r="A51" t="s">
         <v>141</v>
       </c>
@@ -6362,7 +6363,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="52" spans="1:13">
+    <row r="52" spans="1:13" hidden="1">
       <c r="A52" t="s">
         <v>145</v>
       </c>
@@ -6404,7 +6405,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="53" spans="1:13" ht="60">
+    <row r="53" spans="1:13" ht="60" hidden="1">
       <c r="A53" t="s">
         <v>114</v>
       </c>
@@ -6445,7 +6446,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="54" spans="1:13" ht="30">
+    <row r="54" spans="1:13" ht="30" hidden="1">
       <c r="A54" t="s">
         <v>119</v>
       </c>
@@ -6486,7 +6487,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="55" spans="1:13" ht="60">
+    <row r="55" spans="1:13" ht="60" hidden="1">
       <c r="A55" t="s">
         <v>123</v>
       </c>
@@ -6527,7 +6528,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="56" spans="1:13" ht="45">
+    <row r="56" spans="1:13" ht="45" hidden="1">
       <c r="A56" t="s">
         <v>126</v>
       </c>
@@ -6568,7 +6569,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="57" spans="1:13" ht="30">
+    <row r="57" spans="1:13" ht="30" hidden="1">
       <c r="A57" t="s">
         <v>130</v>
       </c>
@@ -6609,7 +6610,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="58" spans="1:13" ht="45">
+    <row r="58" spans="1:13" ht="45" hidden="1">
       <c r="A58" t="s">
         <v>134</v>
       </c>
@@ -6650,7 +6651,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="59" spans="1:13" ht="60">
+    <row r="59" spans="1:13" ht="60" hidden="1">
       <c r="A59" t="s">
         <v>137</v>
       </c>
@@ -6691,7 +6692,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="60" spans="1:13" ht="30">
+    <row r="60" spans="1:13" ht="30" hidden="1">
       <c r="A60" t="s">
         <v>141</v>
       </c>
@@ -6732,7 +6733,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="61" spans="1:13" ht="60">
+    <row r="61" spans="1:13" ht="60" hidden="1">
       <c r="A61" t="s">
         <v>145</v>
       </c>
@@ -6773,7 +6774,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="62" spans="1:13">
+    <row r="62" spans="1:13" hidden="1">
       <c r="A62" t="s">
         <v>181</v>
       </c>
@@ -6815,7 +6816,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="63" spans="1:13">
+    <row r="63" spans="1:13" hidden="1">
       <c r="A63" t="s">
         <v>186</v>
       </c>
@@ -6857,7 +6858,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="64" spans="1:13">
+    <row r="64" spans="1:13" hidden="1">
       <c r="A64" t="s">
         <v>190</v>
       </c>
@@ -6899,7 +6900,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="65" spans="1:13">
+    <row r="65" spans="1:13" hidden="1">
       <c r="A65" t="s">
         <v>194</v>
       </c>
@@ -6941,7 +6942,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="66" spans="1:13">
+    <row r="66" spans="1:13" hidden="1">
       <c r="A66" t="s">
         <v>198</v>
       </c>
@@ -6983,7 +6984,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="67" spans="1:13">
+    <row r="67" spans="1:13" hidden="1">
       <c r="A67" t="s">
         <v>201</v>
       </c>
@@ -7025,7 +7026,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="68" spans="1:13">
+    <row r="68" spans="1:13" hidden="1">
       <c r="A68" t="s">
         <v>181</v>
       </c>
@@ -7067,7 +7068,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="69" spans="1:13">
+    <row r="69" spans="1:13" hidden="1">
       <c r="A69" t="s">
         <v>186</v>
       </c>
@@ -7109,7 +7110,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="70" spans="1:13">
+    <row r="70" spans="1:13" hidden="1">
       <c r="A70" t="s">
         <v>190</v>
       </c>
@@ -7151,7 +7152,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="71" spans="1:13">
+    <row r="71" spans="1:13" hidden="1">
       <c r="A71" t="s">
         <v>194</v>
       </c>
@@ -7193,7 +7194,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="72" spans="1:13">
+    <row r="72" spans="1:13" hidden="1">
       <c r="A72" t="s">
         <v>198</v>
       </c>
@@ -7235,7 +7236,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="73" spans="1:13">
+    <row r="73" spans="1:13" hidden="1">
       <c r="A73" t="s">
         <v>201</v>
       </c>
@@ -7277,7 +7278,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="74" spans="1:13" ht="90">
+    <row r="74" spans="1:13" ht="90" hidden="1">
       <c r="A74" t="s">
         <v>181</v>
       </c>
@@ -7318,7 +7319,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="75" spans="1:13" ht="30">
+    <row r="75" spans="1:13" ht="30" hidden="1">
       <c r="A75" t="s">
         <v>186</v>
       </c>
@@ -7359,7 +7360,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="76" spans="1:13" ht="45">
+    <row r="76" spans="1:13" ht="45" hidden="1">
       <c r="A76" t="s">
         <v>190</v>
       </c>
@@ -7400,7 +7401,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="77" spans="1:13" ht="30">
+    <row r="77" spans="1:13" ht="30" hidden="1">
       <c r="A77" t="s">
         <v>194</v>
       </c>
@@ -7441,7 +7442,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="78" spans="1:13" ht="30">
+    <row r="78" spans="1:13" ht="30" hidden="1">
       <c r="A78" t="s">
         <v>198</v>
       </c>
@@ -7482,7 +7483,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="79" spans="1:13" ht="60">
+    <row r="79" spans="1:13" ht="60" hidden="1">
       <c r="A79" t="s">
         <v>201</v>
       </c>
@@ -7523,7 +7524,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="80" spans="1:13">
+    <row r="80" spans="1:13" hidden="1">
       <c r="A80" t="s">
         <v>229</v>
       </c>
@@ -7565,7 +7566,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="81" spans="1:13">
+    <row r="81" spans="1:13" hidden="1">
       <c r="A81" t="s">
         <v>229</v>
       </c>
@@ -7607,7 +7608,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="82" spans="1:13">
+    <row r="82" spans="1:13" hidden="1">
       <c r="A82" t="s">
         <v>229</v>
       </c>
@@ -7649,7 +7650,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="83" spans="1:13">
+    <row r="83" spans="1:13" hidden="1">
       <c r="A83" t="s">
         <v>237</v>
       </c>
@@ -7691,7 +7692,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="84" spans="1:13">
+    <row r="84" spans="1:13" hidden="1">
       <c r="A84" t="s">
         <v>237</v>
       </c>
@@ -7733,7 +7734,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="85" spans="1:13">
+    <row r="85" spans="1:13" hidden="1">
       <c r="A85" t="s">
         <v>237</v>
       </c>
@@ -7775,7 +7776,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="86" spans="1:13">
+    <row r="86" spans="1:13" hidden="1">
       <c r="A86" t="s">
         <v>245</v>
       </c>
@@ -7817,7 +7818,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="87" spans="1:13">
+    <row r="87" spans="1:13" hidden="1">
       <c r="A87" t="s">
         <v>245</v>
       </c>
@@ -7859,7 +7860,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="88" spans="1:13" ht="30">
+    <row r="88" spans="1:13" ht="30" hidden="1">
       <c r="A88" t="s">
         <v>245</v>
       </c>
@@ -7901,7 +7902,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="89" spans="1:13">
+    <row r="89" spans="1:13" hidden="1">
       <c r="A89" t="s">
         <v>251</v>
       </c>
@@ -7943,7 +7944,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="90" spans="1:13">
+    <row r="90" spans="1:13" hidden="1">
       <c r="A90" t="s">
         <v>251</v>
       </c>
@@ -7985,7 +7986,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="91" spans="1:13" ht="30">
+    <row r="91" spans="1:13" ht="30" hidden="1">
       <c r="A91" t="s">
         <v>251</v>
       </c>
@@ -8027,7 +8028,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="92" spans="1:13">
+    <row r="92" spans="1:13" hidden="1">
       <c r="A92" t="s">
         <v>258</v>
       </c>
@@ -8069,7 +8070,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="93" spans="1:13">
+    <row r="93" spans="1:13" hidden="1">
       <c r="A93" t="s">
         <v>258</v>
       </c>
@@ -8111,7 +8112,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="94" spans="1:13" ht="30">
+    <row r="94" spans="1:13" ht="30" hidden="1">
       <c r="A94" t="s">
         <v>258</v>
       </c>
@@ -8153,7 +8154,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="95" spans="1:13">
+    <row r="95" spans="1:13" hidden="1">
       <c r="A95" t="s">
         <v>264</v>
       </c>
@@ -8195,7 +8196,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="96" spans="1:13">
+    <row r="96" spans="1:13" hidden="1">
       <c r="A96" t="s">
         <v>264</v>
       </c>
@@ -8237,7 +8238,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="97" spans="1:13" ht="30">
+    <row r="97" spans="1:13" ht="30" hidden="1">
       <c r="A97" t="s">
         <v>264</v>
       </c>
@@ -8279,7 +8280,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="98" spans="1:13">
+    <row r="98" spans="1:13" hidden="1">
       <c r="A98" t="s">
         <v>271</v>
       </c>
@@ -8321,7 +8322,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="99" spans="1:13">
+    <row r="99" spans="1:13" hidden="1">
       <c r="A99" t="s">
         <v>271</v>
       </c>
@@ -8363,7 +8364,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="100" spans="1:13" ht="150">
+    <row r="100" spans="1:13" ht="150" hidden="1">
       <c r="A100" t="s">
         <v>271</v>
       </c>
@@ -8405,7 +8406,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="101" spans="1:13">
+    <row r="101" spans="1:13" hidden="1">
       <c r="A101" t="s">
         <v>284</v>
       </c>
@@ -8447,7 +8448,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="102" spans="1:13">
+    <row r="102" spans="1:13" hidden="1">
       <c r="A102" t="s">
         <v>284</v>
       </c>
@@ -8489,7 +8490,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="103" spans="1:13" ht="150">
+    <row r="103" spans="1:13" ht="150" hidden="1">
       <c r="A103" t="s">
         <v>284</v>
       </c>
@@ -8531,7 +8532,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="104" spans="1:13">
+    <row r="104" spans="1:13" hidden="1">
       <c r="A104" t="s">
         <v>291</v>
       </c>
@@ -8573,7 +8574,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="105" spans="1:13">
+    <row r="105" spans="1:13" hidden="1">
       <c r="A105" t="s">
         <v>295</v>
       </c>
@@ -8615,7 +8616,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="106" spans="1:13">
+    <row r="106" spans="1:13" hidden="1">
       <c r="A106" t="s">
         <v>297</v>
       </c>
@@ -8657,7 +8658,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="107" spans="1:13">
+    <row r="107" spans="1:13" hidden="1">
       <c r="A107" t="s">
         <v>299</v>
       </c>
@@ -8699,7 +8700,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="108" spans="1:13">
+    <row r="108" spans="1:13" hidden="1">
       <c r="A108" t="s">
         <v>300</v>
       </c>
@@ -8741,7 +8742,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="109" spans="1:13">
+    <row r="109" spans="1:13" hidden="1">
       <c r="A109" t="s">
         <v>300</v>
       </c>
@@ -8783,7 +8784,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="110" spans="1:13">
+    <row r="110" spans="1:13" hidden="1">
       <c r="A110" t="s">
         <v>300</v>
       </c>
@@ -8825,7 +8826,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="111" spans="1:13">
+    <row r="111" spans="1:13" hidden="1">
       <c r="A111" t="s">
         <v>308</v>
       </c>
@@ -8867,7 +8868,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="112" spans="1:13">
+    <row r="112" spans="1:13" hidden="1">
       <c r="A112" t="s">
         <v>308</v>
       </c>
@@ -8909,7 +8910,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="113" spans="1:13">
+    <row r="113" spans="1:13" hidden="1">
       <c r="A113" t="s">
         <v>308</v>
       </c>
@@ -8951,7 +8952,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="114" spans="1:13">
+    <row r="114" spans="1:13" hidden="1">
       <c r="A114" t="s">
         <v>314</v>
       </c>
@@ -8993,7 +8994,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="115" spans="1:13">
+    <row r="115" spans="1:13" hidden="1">
       <c r="A115" t="s">
         <v>314</v>
       </c>
@@ -9035,7 +9036,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="116" spans="1:13">
+    <row r="116" spans="1:13" hidden="1">
       <c r="A116" t="s">
         <v>314</v>
       </c>
@@ -9077,7 +9078,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="117" spans="1:13">
+    <row r="117" spans="1:13" hidden="1">
       <c r="A117" t="s">
         <v>316</v>
       </c>
@@ -9119,7 +9120,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="118" spans="1:13">
+    <row r="118" spans="1:13" hidden="1">
       <c r="A118" t="s">
         <v>316</v>
       </c>
@@ -9161,7 +9162,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="119" spans="1:13">
+    <row r="119" spans="1:13" hidden="1">
       <c r="A119" t="s">
         <v>316</v>
       </c>
@@ -9203,7 +9204,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="120" spans="1:13">
+    <row r="120" spans="1:13" hidden="1">
       <c r="A120" t="s">
         <v>319</v>
       </c>
@@ -9245,7 +9246,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="121" spans="1:13">
+    <row r="121" spans="1:13" hidden="1">
       <c r="A121" t="s">
         <v>319</v>
       </c>
@@ -9287,7 +9288,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="122" spans="1:13">
+    <row r="122" spans="1:13" hidden="1">
       <c r="A122" t="s">
         <v>319</v>
       </c>
@@ -9329,7 +9330,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="123" spans="1:13">
+    <row r="123" spans="1:13" hidden="1">
       <c r="A123" t="s">
         <v>321</v>
       </c>
@@ -9371,7 +9372,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="124" spans="1:13">
+    <row r="124" spans="1:13" hidden="1">
       <c r="A124" t="s">
         <v>321</v>
       </c>
@@ -9413,7 +9414,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="125" spans="1:13">
+    <row r="125" spans="1:13" hidden="1">
       <c r="A125" t="s">
         <v>321</v>
       </c>
@@ -9455,7 +9456,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="126" spans="1:13">
+    <row r="126" spans="1:13" hidden="1">
       <c r="A126" t="s">
         <v>322</v>
       </c>
@@ -9497,7 +9498,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="127" spans="1:13">
+    <row r="127" spans="1:13" hidden="1">
       <c r="A127" t="s">
         <v>322</v>
       </c>
@@ -9539,7 +9540,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="128" spans="1:13">
+    <row r="128" spans="1:13" hidden="1">
       <c r="A128" t="s">
         <v>322</v>
       </c>
@@ -9581,7 +9582,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="129" spans="1:13">
+    <row r="129" spans="1:13" hidden="1">
       <c r="A129" t="s">
         <v>323</v>
       </c>
@@ -9623,7 +9624,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="130" spans="1:13">
+    <row r="130" spans="1:13" hidden="1">
       <c r="A130" t="s">
         <v>323</v>
       </c>
@@ -9665,7 +9666,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="131" spans="1:13">
+    <row r="131" spans="1:13" hidden="1">
       <c r="A131" t="s">
         <v>323</v>
       </c>
@@ -9707,7 +9708,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="132" spans="1:13">
+    <row r="132" spans="1:13" hidden="1">
       <c r="A132" t="s">
         <v>324</v>
       </c>
@@ -9749,7 +9750,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="133" spans="1:13">
+    <row r="133" spans="1:13" hidden="1">
       <c r="A133" t="s">
         <v>324</v>
       </c>
@@ -9791,7 +9792,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="134" spans="1:13">
+    <row r="134" spans="1:13" hidden="1">
       <c r="A134" t="s">
         <v>324</v>
       </c>
@@ -9833,7 +9834,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="135" spans="1:13">
+    <row r="135" spans="1:13" hidden="1">
       <c r="A135" t="s">
         <v>325</v>
       </c>
@@ -9875,7 +9876,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="136" spans="1:13">
+    <row r="136" spans="1:13" hidden="1">
       <c r="A136" t="s">
         <v>325</v>
       </c>
@@ -9917,7 +9918,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="137" spans="1:13" ht="30">
+    <row r="137" spans="1:13" ht="30" hidden="1">
       <c r="A137" t="s">
         <v>325</v>
       </c>
@@ -9959,7 +9960,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="138" spans="1:13">
+    <row r="138" spans="1:13" hidden="1">
       <c r="A138" t="s">
         <v>333</v>
       </c>
@@ -10001,7 +10002,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="139" spans="1:13">
+    <row r="139" spans="1:13" hidden="1">
       <c r="A139" t="s">
         <v>333</v>
       </c>
@@ -10043,7 +10044,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="140" spans="1:13">
+    <row r="140" spans="1:13" hidden="1">
       <c r="A140" t="s">
         <v>333</v>
       </c>
@@ -10085,7 +10086,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="141" spans="1:13">
+    <row r="141" spans="1:13" hidden="1">
       <c r="A141" t="s">
         <v>341</v>
       </c>
@@ -10127,7 +10128,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="142" spans="1:13">
+    <row r="142" spans="1:13" hidden="1">
       <c r="A142" t="s">
         <v>341</v>
       </c>
@@ -10169,7 +10170,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="143" spans="1:13" ht="30">
+    <row r="143" spans="1:13" ht="30" hidden="1">
       <c r="A143" t="s">
         <v>341</v>
       </c>
@@ -10211,7 +10212,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="144" spans="1:13">
+    <row r="144" spans="1:13" hidden="1">
       <c r="A144" t="s">
         <v>349</v>
       </c>
@@ -10253,7 +10254,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="145" spans="1:13">
+    <row r="145" spans="1:13" hidden="1">
       <c r="A145" t="s">
         <v>349</v>
       </c>
@@ -10295,7 +10296,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="146" spans="1:13" ht="90">
+    <row r="146" spans="1:13" ht="90" hidden="1">
       <c r="A146" t="s">
         <v>349</v>
       </c>
@@ -10337,7 +10338,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="147" spans="1:13">
+    <row r="147" spans="1:13" hidden="1">
       <c r="A147" t="s">
         <v>357</v>
       </c>
@@ -10379,7 +10380,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="148" spans="1:13">
+    <row r="148" spans="1:13" hidden="1">
       <c r="A148" t="s">
         <v>357</v>
       </c>
@@ -10421,7 +10422,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="149" spans="1:13" ht="30">
+    <row r="149" spans="1:13" ht="30" hidden="1">
       <c r="A149" t="s">
         <v>357</v>
       </c>
@@ -10463,7 +10464,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="150" spans="1:13">
+    <row r="150" spans="1:13" hidden="1">
       <c r="A150" t="s">
         <v>364</v>
       </c>
@@ -10505,7 +10506,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="151" spans="1:13">
+    <row r="151" spans="1:13" hidden="1">
       <c r="A151" t="s">
         <v>364</v>
       </c>
@@ -10547,7 +10548,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="152" spans="1:13" ht="30">
+    <row r="152" spans="1:13" ht="30" hidden="1">
       <c r="A152" t="s">
         <v>364</v>
       </c>
@@ -10589,7 +10590,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="153" spans="1:13">
+    <row r="153" spans="1:13" hidden="1">
       <c r="A153" t="s">
         <v>367</v>
       </c>
@@ -10631,7 +10632,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="154" spans="1:13">
+    <row r="154" spans="1:13" hidden="1">
       <c r="A154" t="s">
         <v>367</v>
       </c>
@@ -10673,7 +10674,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="155" spans="1:13" ht="45">
+    <row r="155" spans="1:13" ht="45" hidden="1">
       <c r="A155" t="s">
         <v>367</v>
       </c>
@@ -10715,7 +10716,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="156" spans="1:13">
+    <row r="156" spans="1:13" hidden="1">
       <c r="A156" t="s">
         <v>372</v>
       </c>
@@ -10757,7 +10758,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="157" spans="1:13">
+    <row r="157" spans="1:13" hidden="1">
       <c r="A157" t="s">
         <v>372</v>
       </c>
@@ -10799,7 +10800,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="158" spans="1:13" ht="45">
+    <row r="158" spans="1:13" ht="45" hidden="1">
       <c r="A158" t="s">
         <v>372</v>
       </c>
@@ -10841,7 +10842,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="159" spans="1:13">
+    <row r="159" spans="1:13" hidden="1">
       <c r="A159" t="s">
         <v>374</v>
       </c>
@@ -10883,7 +10884,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="160" spans="1:13">
+    <row r="160" spans="1:13" hidden="1">
       <c r="A160" t="s">
         <v>374</v>
       </c>
@@ -10925,7 +10926,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="161" spans="1:13" ht="60">
+    <row r="161" spans="1:13" ht="60" hidden="1">
       <c r="A161" t="s">
         <v>374</v>
       </c>
@@ -10967,7 +10968,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="162" spans="1:13">
+    <row r="162" spans="1:13" hidden="1">
       <c r="A162" t="s">
         <v>382</v>
       </c>
@@ -11009,7 +11010,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="163" spans="1:13">
+    <row r="163" spans="1:13" hidden="1">
       <c r="A163" t="s">
         <v>382</v>
       </c>
@@ -11051,7 +11052,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="164" spans="1:13" ht="45">
+    <row r="164" spans="1:13" ht="45" hidden="1">
       <c r="A164" t="s">
         <v>382</v>
       </c>
@@ -11093,7 +11094,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="165" spans="1:13">
+    <row r="165" spans="1:13" hidden="1">
       <c r="A165" t="s">
         <v>390</v>
       </c>
@@ -11135,7 +11136,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="166" spans="1:13">
+    <row r="166" spans="1:13" hidden="1">
       <c r="A166" t="s">
         <v>390</v>
       </c>
@@ -11177,7 +11178,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="167" spans="1:13" ht="45">
+    <row r="167" spans="1:13" ht="45" hidden="1">
       <c r="A167" t="s">
         <v>390</v>
       </c>
@@ -11219,7 +11220,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="168" spans="1:13">
+    <row r="168" spans="1:13" hidden="1">
       <c r="A168" t="s">
         <v>398</v>
       </c>
@@ -11261,7 +11262,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="169" spans="1:13">
+    <row r="169" spans="1:13" hidden="1">
       <c r="A169" t="s">
         <v>398</v>
       </c>
@@ -11303,7 +11304,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="170" spans="1:13">
+    <row r="170" spans="1:13" hidden="1">
       <c r="A170" t="s">
         <v>398</v>
       </c>
@@ -11345,7 +11346,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="171" spans="1:13">
+    <row r="171" spans="1:13" hidden="1">
       <c r="A171" t="s">
         <v>405</v>
       </c>
@@ -11387,7 +11388,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="172" spans="1:13">
+    <row r="172" spans="1:13" hidden="1">
       <c r="A172" t="s">
         <v>405</v>
       </c>
@@ -11429,7 +11430,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="173" spans="1:13" ht="30">
+    <row r="173" spans="1:13" ht="30" hidden="1">
       <c r="A173" t="s">
         <v>405</v>
       </c>
@@ -11471,7 +11472,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="174" spans="1:13">
+    <row r="174" spans="1:13" hidden="1">
       <c r="A174" t="s">
         <v>415</v>
       </c>
@@ -11513,7 +11514,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="175" spans="1:13">
+    <row r="175" spans="1:13" hidden="1">
       <c r="A175" t="s">
         <v>415</v>
       </c>
@@ -11555,7 +11556,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="176" spans="1:13" ht="30">
+    <row r="176" spans="1:13" ht="30" hidden="1">
       <c r="A176" t="s">
         <v>415</v>
       </c>
@@ -11597,7 +11598,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="177" spans="1:13">
+    <row r="177" spans="1:13" hidden="1">
       <c r="A177" t="s">
         <v>421</v>
       </c>
@@ -11639,7 +11640,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="178" spans="1:13">
+    <row r="178" spans="1:13" hidden="1">
       <c r="A178" t="s">
         <v>421</v>
       </c>
@@ -11681,7 +11682,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="179" spans="1:13" ht="30">
+    <row r="179" spans="1:13" ht="30" hidden="1">
       <c r="A179" t="s">
         <v>421</v>
       </c>
@@ -11723,7 +11724,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="180" spans="1:13">
+    <row r="180" spans="1:13" hidden="1">
       <c r="A180" t="s">
         <v>429</v>
       </c>
@@ -11765,7 +11766,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="181" spans="1:13">
+    <row r="181" spans="1:13" hidden="1">
       <c r="A181" t="s">
         <v>429</v>
       </c>
@@ -11807,7 +11808,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="182" spans="1:13" ht="30">
+    <row r="182" spans="1:13" ht="30" hidden="1">
       <c r="A182" t="s">
         <v>429</v>
       </c>
@@ -11849,7 +11850,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="183" spans="1:13">
+    <row r="183" spans="1:13" hidden="1">
       <c r="A183" t="s">
         <v>437</v>
       </c>
@@ -11891,7 +11892,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="184" spans="1:13">
+    <row r="184" spans="1:13" hidden="1">
       <c r="A184" t="s">
         <v>437</v>
       </c>
@@ -11933,7 +11934,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="185" spans="1:13" ht="30">
+    <row r="185" spans="1:13" ht="30" hidden="1">
       <c r="A185" t="s">
         <v>437</v>
       </c>
@@ -11975,7 +11976,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="186" spans="1:13">
+    <row r="186" spans="1:13" hidden="1">
       <c r="A186" t="s">
         <v>447</v>
       </c>
@@ -12017,7 +12018,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="187" spans="1:13">
+    <row r="187" spans="1:13" hidden="1">
       <c r="A187" t="s">
         <v>447</v>
       </c>
@@ -12059,7 +12060,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="188" spans="1:13" ht="30">
+    <row r="188" spans="1:13" ht="30" hidden="1">
       <c r="A188" t="s">
         <v>447</v>
       </c>
@@ -12101,7 +12102,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="189" spans="1:13">
+    <row r="189" spans="1:13" hidden="1">
       <c r="A189" t="s">
         <v>452</v>
       </c>
@@ -12143,7 +12144,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="190" spans="1:13">
+    <row r="190" spans="1:13" hidden="1">
       <c r="A190" t="s">
         <v>452</v>
       </c>
@@ -12185,7 +12186,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="191" spans="1:13" ht="30">
+    <row r="191" spans="1:13" ht="30" hidden="1">
       <c r="A191" t="s">
         <v>452</v>
       </c>
@@ -12227,7 +12228,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="192" spans="1:13">
+    <row r="192" spans="1:13" hidden="1">
       <c r="A192" t="s">
         <v>460</v>
       </c>
@@ -12269,7 +12270,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="193" spans="1:13">
+    <row r="193" spans="1:13" hidden="1">
       <c r="A193" t="s">
         <v>460</v>
       </c>
@@ -12311,7 +12312,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="194" spans="1:13" ht="30">
+    <row r="194" spans="1:13" ht="30" hidden="1">
       <c r="A194" t="s">
         <v>460</v>
       </c>
@@ -12353,7 +12354,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="195" spans="1:13">
+    <row r="195" spans="1:13" hidden="1">
       <c r="A195" t="s">
         <v>468</v>
       </c>
@@ -12395,7 +12396,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="196" spans="1:13">
+    <row r="196" spans="1:13" hidden="1">
       <c r="A196" t="s">
         <v>468</v>
       </c>
@@ -12437,7 +12438,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="197" spans="1:13" ht="30">
+    <row r="197" spans="1:13" ht="30" hidden="1">
       <c r="A197" t="s">
         <v>468</v>
       </c>
@@ -12479,7 +12480,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="198" spans="1:13">
+    <row r="198" spans="1:13" hidden="1">
       <c r="A198" t="s">
         <v>473</v>
       </c>
@@ -12521,7 +12522,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="199" spans="1:13">
+    <row r="199" spans="1:13" hidden="1">
       <c r="A199" t="s">
         <v>473</v>
       </c>
@@ -12563,7 +12564,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="200" spans="1:13" ht="30">
+    <row r="200" spans="1:13" ht="30" hidden="1">
       <c r="A200" t="s">
         <v>473</v>
       </c>
@@ -12605,7 +12606,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="201" spans="1:13">
+    <row r="201" spans="1:13" hidden="1">
       <c r="A201" t="s">
         <v>481</v>
       </c>
@@ -12647,7 +12648,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="202" spans="1:13">
+    <row r="202" spans="1:13" hidden="1">
       <c r="A202" t="s">
         <v>481</v>
       </c>
@@ -12689,7 +12690,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="203" spans="1:13" ht="30">
+    <row r="203" spans="1:13" ht="30" hidden="1">
       <c r="A203" t="s">
         <v>481</v>
       </c>
@@ -12731,7 +12732,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="204" spans="1:13">
+    <row r="204" spans="1:13" hidden="1">
       <c r="A204" t="s">
         <v>489</v>
       </c>
@@ -12773,7 +12774,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="205" spans="1:13">
+    <row r="205" spans="1:13" hidden="1">
       <c r="A205" t="s">
         <v>489</v>
       </c>
@@ -12815,7 +12816,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="206" spans="1:13" ht="30">
+    <row r="206" spans="1:13" ht="30" hidden="1">
       <c r="A206" t="s">
         <v>489</v>
       </c>
@@ -12857,7 +12858,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="207" spans="1:13">
+    <row r="207" spans="1:13" hidden="1">
       <c r="A207" t="s">
         <v>494</v>
       </c>
@@ -12899,7 +12900,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="208" spans="1:13">
+    <row r="208" spans="1:13" hidden="1">
       <c r="A208" t="s">
         <v>494</v>
       </c>
@@ -12941,7 +12942,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="209" spans="1:13" ht="30">
+    <row r="209" spans="1:13" ht="30" hidden="1">
       <c r="A209" t="s">
         <v>494</v>
       </c>
@@ -12983,7 +12984,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="210" spans="1:13">
+    <row r="210" spans="1:13" hidden="1">
       <c r="A210" t="s">
         <v>502</v>
       </c>
@@ -13025,7 +13026,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="211" spans="1:13">
+    <row r="211" spans="1:13" hidden="1">
       <c r="A211" t="s">
         <v>502</v>
       </c>
@@ -13067,7 +13068,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="212" spans="1:13">
+    <row r="212" spans="1:13" hidden="1">
       <c r="A212" t="s">
         <v>502</v>
       </c>
@@ -13109,7 +13110,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="213" spans="1:13">
+    <row r="213" spans="1:13" hidden="1">
       <c r="A213" t="s">
         <v>510</v>
       </c>
@@ -13151,7 +13152,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="214" spans="1:13">
+    <row r="214" spans="1:13" hidden="1">
       <c r="A214" t="s">
         <v>510</v>
       </c>
@@ -13193,7 +13194,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="215" spans="1:13" ht="30">
+    <row r="215" spans="1:13" ht="30" hidden="1">
       <c r="A215" t="s">
         <v>510</v>
       </c>
@@ -13235,7 +13236,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="216" spans="1:13">
+    <row r="216" spans="1:13" hidden="1">
       <c r="A216" t="s">
         <v>515</v>
       </c>
@@ -13277,7 +13278,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="217" spans="1:13">
+    <row r="217" spans="1:13" hidden="1">
       <c r="A217" t="s">
         <v>515</v>
       </c>
@@ -13319,7 +13320,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="218" spans="1:13" ht="30">
+    <row r="218" spans="1:13" ht="30" hidden="1">
       <c r="A218" t="s">
         <v>515</v>
       </c>
@@ -13361,7 +13362,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="219" spans="1:13">
+    <row r="219" spans="1:13" hidden="1">
       <c r="A219" t="s">
         <v>523</v>
       </c>
@@ -13403,7 +13404,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="220" spans="1:13">
+    <row r="220" spans="1:13" hidden="1">
       <c r="A220" t="s">
         <v>523</v>
       </c>
@@ -13445,7 +13446,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="221" spans="1:13">
+    <row r="221" spans="1:13" hidden="1">
       <c r="A221" t="s">
         <v>523</v>
       </c>
@@ -13487,7 +13488,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="222" spans="1:13">
+    <row r="222" spans="1:13" hidden="1">
       <c r="A222" t="s">
         <v>531</v>
       </c>
@@ -13529,7 +13530,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="223" spans="1:13">
+    <row r="223" spans="1:13" hidden="1">
       <c r="A223" t="s">
         <v>531</v>
       </c>
@@ -13571,7 +13572,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="224" spans="1:13" ht="30">
+    <row r="224" spans="1:13" ht="30" hidden="1">
       <c r="A224" t="s">
         <v>531</v>
       </c>
@@ -13613,7 +13614,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="225" spans="1:13">
+    <row r="225" spans="1:13" hidden="1">
       <c r="A225" t="s">
         <v>536</v>
       </c>
@@ -13655,7 +13656,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="226" spans="1:13">
+    <row r="226" spans="1:13" hidden="1">
       <c r="A226" t="s">
         <v>536</v>
       </c>
@@ -13697,7 +13698,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="227" spans="1:13" ht="30">
+    <row r="227" spans="1:13" ht="30" hidden="1">
       <c r="A227" t="s">
         <v>536</v>
       </c>
@@ -13739,7 +13740,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="228" spans="1:13">
+    <row r="228" spans="1:13" hidden="1">
       <c r="A228" t="s">
         <v>544</v>
       </c>
@@ -13781,7 +13782,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="229" spans="1:13">
+    <row r="229" spans="1:13" hidden="1">
       <c r="A229" t="s">
         <v>544</v>
       </c>
@@ -13823,7 +13824,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="230" spans="1:13">
+    <row r="230" spans="1:13" hidden="1">
       <c r="A230" t="s">
         <v>544</v>
       </c>
@@ -13865,7 +13866,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="231" spans="1:13">
+    <row r="231" spans="1:13" hidden="1">
       <c r="A231" t="s">
         <v>552</v>
       </c>
@@ -13907,7 +13908,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="232" spans="1:13">
+    <row r="232" spans="1:13" hidden="1">
       <c r="A232" t="s">
         <v>552</v>
       </c>
@@ -13949,7 +13950,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="233" spans="1:13" ht="30">
+    <row r="233" spans="1:13" ht="30" hidden="1">
       <c r="A233" t="s">
         <v>552</v>
       </c>
@@ -13991,7 +13992,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="234" spans="1:13">
+    <row r="234" spans="1:13" hidden="1">
       <c r="A234" t="s">
         <v>557</v>
       </c>
@@ -14033,7 +14034,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="235" spans="1:13">
+    <row r="235" spans="1:13" hidden="1">
       <c r="A235" t="s">
         <v>557</v>
       </c>
@@ -14075,7 +14076,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="236" spans="1:13" ht="30">
+    <row r="236" spans="1:13" ht="30" hidden="1">
       <c r="A236" t="s">
         <v>557</v>
       </c>
@@ -14117,7 +14118,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="237" spans="1:13">
+    <row r="237" spans="1:13" hidden="1">
       <c r="A237" t="s">
         <v>565</v>
       </c>
@@ -14159,7 +14160,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="238" spans="1:13">
+    <row r="238" spans="1:13" hidden="1">
       <c r="A238" t="s">
         <v>565</v>
       </c>
@@ -14201,7 +14202,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="239" spans="1:13" ht="30">
+    <row r="239" spans="1:13" ht="30" hidden="1">
       <c r="A239" t="s">
         <v>565</v>
       </c>
@@ -14243,7 +14244,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="240" spans="1:13">
+    <row r="240" spans="1:13" hidden="1">
       <c r="A240" t="s">
         <v>573</v>
       </c>
@@ -14285,7 +14286,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="241" spans="1:13">
+    <row r="241" spans="1:13" hidden="1">
       <c r="A241" t="s">
         <v>573</v>
       </c>
@@ -14327,7 +14328,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="242" spans="1:13" ht="30">
+    <row r="242" spans="1:13" ht="30" hidden="1">
       <c r="A242" t="s">
         <v>573</v>
       </c>
@@ -14369,7 +14370,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="243" spans="1:13">
+    <row r="243" spans="1:13" hidden="1">
       <c r="A243" t="s">
         <v>580</v>
       </c>
@@ -14411,7 +14412,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="244" spans="1:13">
+    <row r="244" spans="1:13" hidden="1">
       <c r="A244" t="s">
         <v>580</v>
       </c>
@@ -14453,7 +14454,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="245" spans="1:13" ht="30">
+    <row r="245" spans="1:13" ht="30" hidden="1">
       <c r="A245" t="s">
         <v>580</v>
       </c>
@@ -14495,7 +14496,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="246" spans="1:13">
+    <row r="246" spans="1:13" hidden="1">
       <c r="A246" t="s">
         <v>588</v>
       </c>
@@ -14537,7 +14538,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="247" spans="1:13">
+    <row r="247" spans="1:13" hidden="1">
       <c r="A247" t="s">
         <v>588</v>
       </c>
@@ -14579,7 +14580,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="248" spans="1:13" ht="30">
+    <row r="248" spans="1:13" ht="30" hidden="1">
       <c r="A248" t="s">
         <v>588</v>
       </c>
@@ -14621,7 +14622,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="249" spans="1:13">
+    <row r="249" spans="1:13" hidden="1">
       <c r="A249" t="s">
         <v>596</v>
       </c>
@@ -14663,7 +14664,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="250" spans="1:13">
+    <row r="250" spans="1:13" hidden="1">
       <c r="A250" t="s">
         <v>596</v>
       </c>
@@ -14705,7 +14706,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="251" spans="1:13" ht="30">
+    <row r="251" spans="1:13" ht="30" hidden="1">
       <c r="A251" t="s">
         <v>596</v>
       </c>
@@ -14747,7 +14748,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="252" spans="1:13">
+    <row r="252" spans="1:13" hidden="1">
       <c r="A252" t="s">
         <v>601</v>
       </c>
@@ -14789,7 +14790,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="253" spans="1:13">
+    <row r="253" spans="1:13" hidden="1">
       <c r="A253" t="s">
         <v>601</v>
       </c>
@@ -14831,7 +14832,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="254" spans="1:13" ht="30">
+    <row r="254" spans="1:13" ht="30" hidden="1">
       <c r="A254" t="s">
         <v>601</v>
       </c>
@@ -14873,7 +14874,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="255" spans="1:13">
+    <row r="255" spans="1:13" hidden="1">
       <c r="A255" t="s">
         <v>609</v>
       </c>
@@ -14915,7 +14916,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="256" spans="1:13">
+    <row r="256" spans="1:13" hidden="1">
       <c r="A256" t="s">
         <v>609</v>
       </c>
@@ -14957,7 +14958,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="257" spans="1:13" ht="30">
+    <row r="257" spans="1:13" ht="30" hidden="1">
       <c r="A257" t="s">
         <v>609</v>
       </c>
@@ -14999,7 +15000,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="258" spans="1:13">
+    <row r="258" spans="1:13" hidden="1">
       <c r="A258" t="s">
         <v>617</v>
       </c>
@@ -15041,7 +15042,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="259" spans="1:13">
+    <row r="259" spans="1:13" hidden="1">
       <c r="A259" t="s">
         <v>617</v>
       </c>
@@ -15083,7 +15084,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="260" spans="1:13" ht="30">
+    <row r="260" spans="1:13" ht="30" hidden="1">
       <c r="A260" t="s">
         <v>617</v>
       </c>
@@ -15125,7 +15126,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="261" spans="1:13">
+    <row r="261" spans="1:13" hidden="1">
       <c r="A261" t="s">
         <v>622</v>
       </c>
@@ -15167,7 +15168,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="262" spans="1:13">
+    <row r="262" spans="1:13" hidden="1">
       <c r="A262" t="s">
         <v>622</v>
       </c>
@@ -15209,7 +15210,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="263" spans="1:13" ht="30">
+    <row r="263" spans="1:13" ht="30" hidden="1">
       <c r="A263" t="s">
         <v>622</v>
       </c>
@@ -15251,7 +15252,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="264" spans="1:13">
+    <row r="264" spans="1:13" hidden="1">
       <c r="A264" t="s">
         <v>630</v>
       </c>
@@ -15293,7 +15294,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="265" spans="1:13">
+    <row r="265" spans="1:13" hidden="1">
       <c r="A265" t="s">
         <v>630</v>
       </c>
@@ -15335,7 +15336,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="266" spans="1:13" ht="30">
+    <row r="266" spans="1:13" ht="30" hidden="1">
       <c r="A266" t="s">
         <v>630</v>
       </c>
@@ -15377,7 +15378,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="267" spans="1:13">
+    <row r="267" spans="1:13" hidden="1">
       <c r="A267" t="s">
         <v>638</v>
       </c>
@@ -15419,7 +15420,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="268" spans="1:13">
+    <row r="268" spans="1:13" hidden="1">
       <c r="A268" t="s">
         <v>638</v>
       </c>
@@ -15461,7 +15462,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="269" spans="1:13" ht="30">
+    <row r="269" spans="1:13" ht="30" hidden="1">
       <c r="A269" t="s">
         <v>638</v>
       </c>
@@ -15503,7 +15504,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="270" spans="1:13">
+    <row r="270" spans="1:13" hidden="1">
       <c r="A270" t="s">
         <v>643</v>
       </c>
@@ -15545,7 +15546,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="271" spans="1:13">
+    <row r="271" spans="1:13" hidden="1">
       <c r="A271" t="s">
         <v>643</v>
       </c>
@@ -15587,7 +15588,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="272" spans="1:13" ht="30">
+    <row r="272" spans="1:13" ht="30" hidden="1">
       <c r="A272" t="s">
         <v>643</v>
       </c>
@@ -15629,7 +15630,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="273" spans="1:13">
+    <row r="273" spans="1:13" hidden="1">
       <c r="A273" t="s">
         <v>651</v>
       </c>
@@ -15671,7 +15672,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="274" spans="1:13">
+    <row r="274" spans="1:13" hidden="1">
       <c r="A274" t="s">
         <v>651</v>
       </c>
@@ -15713,7 +15714,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="275" spans="1:13" ht="30">
+    <row r="275" spans="1:13" ht="30" hidden="1">
       <c r="A275" t="s">
         <v>651</v>
       </c>
@@ -15755,7 +15756,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="276" spans="1:13">
+    <row r="276" spans="1:13" hidden="1">
       <c r="A276" t="s">
         <v>659</v>
       </c>
@@ -15797,7 +15798,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="277" spans="1:13">
+    <row r="277" spans="1:13" hidden="1">
       <c r="A277" t="s">
         <v>659</v>
       </c>
@@ -15839,7 +15840,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="278" spans="1:13" ht="30">
+    <row r="278" spans="1:13" ht="30" hidden="1">
       <c r="A278" t="s">
         <v>659</v>
       </c>
@@ -15881,7 +15882,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="279" spans="1:13">
+    <row r="279" spans="1:13" hidden="1">
       <c r="A279" t="s">
         <v>664</v>
       </c>
@@ -15923,7 +15924,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="280" spans="1:13">
+    <row r="280" spans="1:13" hidden="1">
       <c r="A280" t="s">
         <v>664</v>
       </c>
@@ -15965,7 +15966,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="281" spans="1:13" ht="30">
+    <row r="281" spans="1:13" ht="30" hidden="1">
       <c r="A281" t="s">
         <v>664</v>
       </c>
@@ -16007,7 +16008,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="282" spans="1:13">
+    <row r="282" spans="1:13" hidden="1">
       <c r="A282" t="s">
         <v>672</v>
       </c>
@@ -16049,7 +16050,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="283" spans="1:13">
+    <row r="283" spans="1:13" hidden="1">
       <c r="A283" t="s">
         <v>672</v>
       </c>
@@ -16091,7 +16092,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="284" spans="1:13" ht="30">
+    <row r="284" spans="1:13" ht="30" hidden="1">
       <c r="A284" t="s">
         <v>672</v>
       </c>
@@ -16133,7 +16134,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="285" spans="1:13">
+    <row r="285" spans="1:13" hidden="1">
       <c r="A285" t="s">
         <v>678</v>
       </c>
@@ -16175,7 +16176,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="286" spans="1:13">
+    <row r="286" spans="1:13" hidden="1">
       <c r="A286" t="s">
         <v>678</v>
       </c>
@@ -16217,7 +16218,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="287" spans="1:13" ht="30">
+    <row r="287" spans="1:13" ht="30" hidden="1">
       <c r="A287" t="s">
         <v>678</v>
       </c>
@@ -16259,7 +16260,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="288" spans="1:13">
+    <row r="288" spans="1:13" hidden="1">
       <c r="A288" t="s">
         <v>683</v>
       </c>
@@ -16301,7 +16302,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="289" spans="1:13">
+    <row r="289" spans="1:13" hidden="1">
       <c r="A289" t="s">
         <v>683</v>
       </c>
@@ -16343,7 +16344,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="290" spans="1:13" ht="30">
+    <row r="290" spans="1:13" ht="30" hidden="1">
       <c r="A290" t="s">
         <v>683</v>
       </c>
@@ -16385,7 +16386,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="291" spans="1:13">
+    <row r="291" spans="1:13" hidden="1">
       <c r="A291" t="s">
         <v>691</v>
       </c>
@@ -16427,7 +16428,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="292" spans="1:13">
+    <row r="292" spans="1:13" hidden="1">
       <c r="A292" t="s">
         <v>691</v>
       </c>
@@ -16469,7 +16470,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="293" spans="1:13">
+    <row r="293" spans="1:13" hidden="1">
       <c r="A293" t="s">
         <v>691</v>
       </c>
@@ -16511,7 +16512,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="294" spans="1:13">
+    <row r="294" spans="1:13" hidden="1">
       <c r="A294" t="s">
         <v>699</v>
       </c>
@@ -16553,7 +16554,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="295" spans="1:13">
+    <row r="295" spans="1:13" hidden="1">
       <c r="A295" t="s">
         <v>699</v>
       </c>
@@ -16595,7 +16596,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="296" spans="1:13" ht="30">
+    <row r="296" spans="1:13" ht="30" hidden="1">
       <c r="A296" t="s">
         <v>699</v>
       </c>
@@ -16637,7 +16638,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="297" spans="1:13">
+    <row r="297" spans="1:13" hidden="1">
       <c r="A297" t="s">
         <v>704</v>
       </c>
@@ -16679,7 +16680,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="298" spans="1:13">
+    <row r="298" spans="1:13" hidden="1">
       <c r="A298" t="s">
         <v>704</v>
       </c>
@@ -16721,7 +16722,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="299" spans="1:13" ht="30">
+    <row r="299" spans="1:13" ht="30" hidden="1">
       <c r="A299" t="s">
         <v>704</v>
       </c>
@@ -16763,7 +16764,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="300" spans="1:13">
+    <row r="300" spans="1:13" hidden="1">
       <c r="A300" t="s">
         <v>712</v>
       </c>
@@ -16805,7 +16806,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="301" spans="1:13">
+    <row r="301" spans="1:13" hidden="1">
       <c r="A301" t="s">
         <v>712</v>
       </c>
@@ -16847,7 +16848,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="302" spans="1:13" ht="30">
+    <row r="302" spans="1:13" ht="30" hidden="1">
       <c r="A302" t="s">
         <v>712</v>
       </c>
@@ -16889,7 +16890,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="303" spans="1:13">
+    <row r="303" spans="1:13" hidden="1">
       <c r="A303" t="s">
         <v>720</v>
       </c>
@@ -16931,7 +16932,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="304" spans="1:13">
+    <row r="304" spans="1:13" hidden="1">
       <c r="A304" t="s">
         <v>720</v>
       </c>
@@ -16973,7 +16974,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="305" spans="1:13" ht="30">
+    <row r="305" spans="1:13" ht="30" hidden="1">
       <c r="A305" t="s">
         <v>720</v>
       </c>
@@ -17015,7 +17016,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="306" spans="1:13">
+    <row r="306" spans="1:13" hidden="1">
       <c r="A306" t="s">
         <v>725</v>
       </c>
@@ -17057,7 +17058,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="307" spans="1:13">
+    <row r="307" spans="1:13" hidden="1">
       <c r="A307" t="s">
         <v>725</v>
       </c>
@@ -17099,7 +17100,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="308" spans="1:13" ht="30">
+    <row r="308" spans="1:13" ht="30" hidden="1">
       <c r="A308" t="s">
         <v>725</v>
       </c>
@@ -17141,7 +17142,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="309" spans="1:13">
+    <row r="309" spans="1:13" hidden="1">
       <c r="A309" t="s">
         <v>733</v>
       </c>
@@ -17183,7 +17184,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="310" spans="1:13">
+    <row r="310" spans="1:13" hidden="1">
       <c r="A310" t="s">
         <v>733</v>
       </c>
@@ -17225,7 +17226,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="311" spans="1:13" ht="30">
+    <row r="311" spans="1:13" ht="30" hidden="1">
       <c r="A311" t="s">
         <v>733</v>
       </c>
@@ -17267,7 +17268,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="312" spans="1:13">
+    <row r="312" spans="1:13" hidden="1">
       <c r="A312" t="s">
         <v>741</v>
       </c>
@@ -17309,7 +17310,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="313" spans="1:13">
+    <row r="313" spans="1:13" hidden="1">
       <c r="A313" t="s">
         <v>741</v>
       </c>
@@ -17351,7 +17352,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="314" spans="1:13" ht="30">
+    <row r="314" spans="1:13" ht="30" hidden="1">
       <c r="A314" t="s">
         <v>741</v>
       </c>
@@ -17393,7 +17394,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="315" spans="1:13">
+    <row r="315" spans="1:13" hidden="1">
       <c r="A315" t="s">
         <v>746</v>
       </c>
@@ -17435,7 +17436,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="316" spans="1:13">
+    <row r="316" spans="1:13" hidden="1">
       <c r="A316" t="s">
         <v>746</v>
       </c>
@@ -17477,7 +17478,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="317" spans="1:13" ht="30">
+    <row r="317" spans="1:13" ht="30" hidden="1">
       <c r="A317" t="s">
         <v>746</v>
       </c>
@@ -17519,7 +17520,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="318" spans="1:13">
+    <row r="318" spans="1:13" hidden="1">
       <c r="A318" t="s">
         <v>753</v>
       </c>
@@ -17561,7 +17562,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="319" spans="1:13">
+    <row r="319" spans="1:13" hidden="1">
       <c r="A319" t="s">
         <v>753</v>
       </c>
@@ -17603,7 +17604,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="320" spans="1:13" ht="30">
+    <row r="320" spans="1:13" ht="30" hidden="1">
       <c r="A320" t="s">
         <v>753</v>
       </c>
@@ -17645,7 +17646,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="321" spans="1:13">
+    <row r="321" spans="1:13" hidden="1">
       <c r="A321" t="s">
         <v>757</v>
       </c>
@@ -17687,7 +17688,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="322" spans="1:13">
+    <row r="322" spans="1:13" hidden="1">
       <c r="A322" t="s">
         <v>757</v>
       </c>
@@ -17729,7 +17730,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="323" spans="1:13" ht="30">
+    <row r="323" spans="1:13" ht="30" hidden="1">
       <c r="A323" t="s">
         <v>757</v>
       </c>
@@ -17771,7 +17772,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="324" spans="1:13">
+    <row r="324" spans="1:13" hidden="1">
       <c r="A324" t="s">
         <v>764</v>
       </c>
@@ -17813,7 +17814,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="325" spans="1:13">
+    <row r="325" spans="1:13" hidden="1">
       <c r="A325" t="s">
         <v>764</v>
       </c>
@@ -17855,7 +17856,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="326" spans="1:13" ht="30">
+    <row r="326" spans="1:13" ht="30" hidden="1">
       <c r="A326" t="s">
         <v>764</v>
       </c>
@@ -17897,7 +17898,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="327" spans="1:13">
+    <row r="327" spans="1:13" hidden="1">
       <c r="A327" t="s">
         <v>768</v>
       </c>
@@ -17939,7 +17940,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="328" spans="1:13">
+    <row r="328" spans="1:13" hidden="1">
       <c r="A328" t="s">
         <v>768</v>
       </c>
@@ -17981,7 +17982,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="329" spans="1:13" ht="30">
+    <row r="329" spans="1:13" ht="30" hidden="1">
       <c r="A329" t="s">
         <v>768</v>
       </c>
@@ -18023,7 +18024,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="330" spans="1:13">
+    <row r="330" spans="1:13" hidden="1">
       <c r="A330" t="s">
         <v>775</v>
       </c>
@@ -18065,7 +18066,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="331" spans="1:13">
+    <row r="331" spans="1:13" hidden="1">
       <c r="A331" t="s">
         <v>775</v>
       </c>
@@ -18107,7 +18108,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="332" spans="1:13" ht="30">
+    <row r="332" spans="1:13" ht="30" hidden="1">
       <c r="A332" t="s">
         <v>775</v>
       </c>
@@ -18149,7 +18150,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="333" spans="1:13">
+    <row r="333" spans="1:13" hidden="1">
       <c r="A333" t="s">
         <v>779</v>
       </c>
@@ -18191,7 +18192,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="334" spans="1:13">
+    <row r="334" spans="1:13" hidden="1">
       <c r="A334" t="s">
         <v>779</v>
       </c>
@@ -18233,7 +18234,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="335" spans="1:13" ht="30">
+    <row r="335" spans="1:13" ht="30" hidden="1">
       <c r="A335" t="s">
         <v>779</v>
       </c>
@@ -18275,7 +18276,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="336" spans="1:13">
+    <row r="336" spans="1:13" hidden="1">
       <c r="A336" t="s">
         <v>783</v>
       </c>
@@ -18317,7 +18318,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="337" spans="1:13">
+    <row r="337" spans="1:13" hidden="1">
       <c r="A337" t="s">
         <v>783</v>
       </c>
@@ -18359,7 +18360,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="338" spans="1:13" ht="30">
+    <row r="338" spans="1:13" ht="30" hidden="1">
       <c r="A338" t="s">
         <v>783</v>
       </c>
@@ -18401,7 +18402,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="339" spans="1:13">
+    <row r="339" spans="1:13" hidden="1">
       <c r="A339" t="s">
         <v>787</v>
       </c>
@@ -18443,7 +18444,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="340" spans="1:13">
+    <row r="340" spans="1:13" hidden="1">
       <c r="A340" t="s">
         <v>787</v>
       </c>
@@ -18485,7 +18486,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="341" spans="1:13" ht="30">
+    <row r="341" spans="1:13" ht="30" hidden="1">
       <c r="A341" t="s">
         <v>787</v>
       </c>
@@ -18527,7 +18528,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="342" spans="1:13">
+    <row r="342" spans="1:13" hidden="1">
       <c r="A342" t="s">
         <v>794</v>
       </c>
@@ -18569,7 +18570,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="343" spans="1:13">
+    <row r="343" spans="1:13" hidden="1">
       <c r="A343" t="s">
         <v>794</v>
       </c>
@@ -18611,7 +18612,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="344" spans="1:13" ht="30">
+    <row r="344" spans="1:13" ht="30" hidden="1">
       <c r="A344" t="s">
         <v>794</v>
       </c>
@@ -18653,7 +18654,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="345" spans="1:13">
+    <row r="345" spans="1:13" hidden="1">
       <c r="A345" t="s">
         <v>798</v>
       </c>
@@ -18695,7 +18696,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="346" spans="1:13">
+    <row r="346" spans="1:13" hidden="1">
       <c r="A346" t="s">
         <v>798</v>
       </c>
@@ -18737,7 +18738,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="347" spans="1:13" ht="30">
+    <row r="347" spans="1:13" ht="30" hidden="1">
       <c r="A347" t="s">
         <v>798</v>
       </c>
@@ -18779,7 +18780,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="348" spans="1:13">
+    <row r="348" spans="1:13" hidden="1">
       <c r="A348" t="s">
         <v>805</v>
       </c>
@@ -18821,7 +18822,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="349" spans="1:13">
+    <row r="349" spans="1:13" hidden="1">
       <c r="A349" t="s">
         <v>805</v>
       </c>
@@ -18863,7 +18864,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="350" spans="1:13" ht="30">
+    <row r="350" spans="1:13" ht="30" hidden="1">
       <c r="A350" t="s">
         <v>805</v>
       </c>
@@ -18905,7 +18906,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="351" spans="1:13">
+    <row r="351" spans="1:13" hidden="1">
       <c r="A351" t="s">
         <v>809</v>
       </c>
@@ -18947,7 +18948,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="352" spans="1:13">
+    <row r="352" spans="1:13" hidden="1">
       <c r="A352" t="s">
         <v>809</v>
       </c>
@@ -18989,7 +18990,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="353" spans="1:13" ht="30">
+    <row r="353" spans="1:13" ht="30" hidden="1">
       <c r="A353" t="s">
         <v>809</v>
       </c>
@@ -19031,7 +19032,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="354" spans="1:13">
+    <row r="354" spans="1:13" hidden="1">
       <c r="A354" t="s">
         <v>816</v>
       </c>
@@ -19073,7 +19074,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="355" spans="1:13">
+    <row r="355" spans="1:13" hidden="1">
       <c r="A355" t="s">
         <v>816</v>
       </c>
@@ -19115,7 +19116,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="356" spans="1:13" ht="30">
+    <row r="356" spans="1:13" ht="30" hidden="1">
       <c r="A356" t="s">
         <v>816</v>
       </c>
@@ -19157,7 +19158,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="357" spans="1:13">
+    <row r="357" spans="1:13" hidden="1">
       <c r="A357" t="s">
         <v>820</v>
       </c>
@@ -19199,7 +19200,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="358" spans="1:13">
+    <row r="358" spans="1:13" hidden="1">
       <c r="A358" t="s">
         <v>820</v>
       </c>
@@ -19241,7 +19242,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="359" spans="1:13" ht="30">
+    <row r="359" spans="1:13" ht="30" hidden="1">
       <c r="A359" t="s">
         <v>820</v>
       </c>
@@ -19283,7 +19284,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="360" spans="1:13">
+    <row r="360" spans="1:13" hidden="1">
       <c r="A360" t="s">
         <v>826</v>
       </c>
@@ -19325,7 +19326,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="361" spans="1:13">
+    <row r="361" spans="1:13" hidden="1">
       <c r="A361" t="s">
         <v>826</v>
       </c>
@@ -19367,7 +19368,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="362" spans="1:13" ht="30">
+    <row r="362" spans="1:13" ht="30" hidden="1">
       <c r="A362" t="s">
         <v>826</v>
       </c>
@@ -19409,7 +19410,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="363" spans="1:13">
+    <row r="363" spans="1:13" hidden="1">
       <c r="A363" t="s">
         <v>833</v>
       </c>
@@ -19451,7 +19452,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="364" spans="1:13">
+    <row r="364" spans="1:13" hidden="1">
       <c r="A364" t="s">
         <v>833</v>
       </c>
@@ -19493,7 +19494,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="365" spans="1:13" ht="30">
+    <row r="365" spans="1:13" ht="30" hidden="1">
       <c r="A365" t="s">
         <v>833</v>
       </c>
@@ -19535,7 +19536,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="366" spans="1:13">
+    <row r="366" spans="1:13" hidden="1">
       <c r="A366" t="s">
         <v>840</v>
       </c>
@@ -19577,7 +19578,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="367" spans="1:13">
+    <row r="367" spans="1:13" hidden="1">
       <c r="A367" t="s">
         <v>840</v>
       </c>
@@ -19619,7 +19620,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="368" spans="1:13" ht="30">
+    <row r="368" spans="1:13" ht="30" hidden="1">
       <c r="A368" t="s">
         <v>840</v>
       </c>
@@ -19661,7 +19662,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="369" spans="1:13">
+    <row r="369" spans="1:13" hidden="1">
       <c r="A369" t="s">
         <v>847</v>
       </c>
@@ -19703,7 +19704,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="370" spans="1:13">
+    <row r="370" spans="1:13" hidden="1">
       <c r="A370" t="s">
         <v>847</v>
       </c>
@@ -19745,7 +19746,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="371" spans="1:13" ht="30">
+    <row r="371" spans="1:13" ht="30" hidden="1">
       <c r="A371" t="s">
         <v>847</v>
       </c>
@@ -19787,7 +19788,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="372" spans="1:13">
+    <row r="372" spans="1:13" hidden="1">
       <c r="A372" t="s">
         <v>851</v>
       </c>
@@ -19829,7 +19830,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="373" spans="1:13">
+    <row r="373" spans="1:13" hidden="1">
       <c r="A373" t="s">
         <v>851</v>
       </c>
@@ -19871,7 +19872,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="374" spans="1:13" ht="30">
+    <row r="374" spans="1:13" ht="30" hidden="1">
       <c r="A374" t="s">
         <v>851</v>
       </c>
@@ -19913,7 +19914,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="375" spans="1:13">
+    <row r="375" spans="1:13" hidden="1">
       <c r="A375" t="s">
         <v>858</v>
       </c>
@@ -19955,7 +19956,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="376" spans="1:13">
+    <row r="376" spans="1:13" hidden="1">
       <c r="A376" t="s">
         <v>858</v>
       </c>
@@ -19997,7 +19998,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="377" spans="1:13" ht="30">
+    <row r="377" spans="1:13" ht="30" hidden="1">
       <c r="A377" t="s">
         <v>858</v>
       </c>
@@ -20039,7 +20040,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="378" spans="1:13">
+    <row r="378" spans="1:13" hidden="1">
       <c r="A378" t="s">
         <v>865</v>
       </c>
@@ -20081,7 +20082,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="379" spans="1:13">
+    <row r="379" spans="1:13" hidden="1">
       <c r="A379" t="s">
         <v>865</v>
       </c>
@@ -20123,7 +20124,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="380" spans="1:13" ht="60">
+    <row r="380" spans="1:13" ht="60" hidden="1">
       <c r="A380" t="s">
         <v>865</v>
       </c>
@@ -20165,7 +20166,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="381" spans="1:13">
+    <row r="381" spans="1:13" hidden="1">
       <c r="A381" t="s">
         <v>872</v>
       </c>
@@ -20207,7 +20208,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="382" spans="1:13">
+    <row r="382" spans="1:13" hidden="1">
       <c r="A382" t="s">
         <v>872</v>
       </c>
@@ -20249,7 +20250,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="383" spans="1:13" ht="60">
+    <row r="383" spans="1:13" ht="60" hidden="1">
       <c r="A383" t="s">
         <v>872</v>
       </c>
@@ -20291,7 +20292,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="384" spans="1:13">
+    <row r="384" spans="1:13" hidden="1">
       <c r="A384" t="s">
         <v>876</v>
       </c>
@@ -20333,7 +20334,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="385" spans="1:13">
+    <row r="385" spans="1:13" hidden="1">
       <c r="A385" t="s">
         <v>876</v>
       </c>
@@ -20375,7 +20376,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="386" spans="1:13" ht="30">
+    <row r="386" spans="1:13" ht="30" hidden="1">
       <c r="A386" t="s">
         <v>876</v>
       </c>
@@ -20417,7 +20418,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="387" spans="1:13">
+    <row r="387" spans="1:13" hidden="1">
       <c r="A387" t="s">
         <v>883</v>
       </c>
@@ -20459,7 +20460,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="388" spans="1:13">
+    <row r="388" spans="1:13" hidden="1">
       <c r="A388" t="s">
         <v>883</v>
       </c>
@@ -20501,7 +20502,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="389" spans="1:13" ht="30">
+    <row r="389" spans="1:13" ht="30" hidden="1">
       <c r="A389" t="s">
         <v>883</v>
       </c>
@@ -20543,7 +20544,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="390" spans="1:13">
+    <row r="390" spans="1:13" hidden="1">
       <c r="A390" t="s">
         <v>890</v>
       </c>
@@ -20585,7 +20586,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="391" spans="1:13">
+    <row r="391" spans="1:13" hidden="1">
       <c r="A391" t="s">
         <v>890</v>
       </c>
@@ -20627,7 +20628,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="392" spans="1:13" ht="30">
+    <row r="392" spans="1:13" ht="30" hidden="1">
       <c r="A392" t="s">
         <v>890</v>
       </c>
@@ -20669,7 +20670,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="393" spans="1:13">
+    <row r="393" spans="1:13" hidden="1">
       <c r="A393" t="s">
         <v>894</v>
       </c>
@@ -20711,7 +20712,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="394" spans="1:13">
+    <row r="394" spans="1:13" hidden="1">
       <c r="A394" t="s">
         <v>894</v>
       </c>
@@ -20753,7 +20754,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="395" spans="1:13" ht="30">
+    <row r="395" spans="1:13" ht="30" hidden="1">
       <c r="A395" t="s">
         <v>894</v>
       </c>
@@ -20795,7 +20796,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="396" spans="1:13">
+    <row r="396" spans="1:13" hidden="1">
       <c r="A396" t="s">
         <v>901</v>
       </c>
@@ -20837,7 +20838,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="397" spans="1:13">
+    <row r="397" spans="1:13" hidden="1">
       <c r="A397" t="s">
         <v>901</v>
       </c>
@@ -20879,7 +20880,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="398" spans="1:13" ht="30">
+    <row r="398" spans="1:13" ht="30" hidden="1">
       <c r="A398" t="s">
         <v>901</v>
       </c>
@@ -20921,7 +20922,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="399" spans="1:13">
+    <row r="399" spans="1:13" hidden="1">
       <c r="A399" t="s">
         <v>908</v>
       </c>
@@ -20963,7 +20964,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="400" spans="1:13">
+    <row r="400" spans="1:13" hidden="1">
       <c r="A400" t="s">
         <v>908</v>
       </c>
@@ -21005,7 +21006,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="401" spans="1:13" ht="30">
+    <row r="401" spans="1:13" ht="30" hidden="1">
       <c r="A401" t="s">
         <v>908</v>
       </c>
@@ -21047,7 +21048,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="402" spans="1:13">
+    <row r="402" spans="1:13" hidden="1">
       <c r="A402" t="s">
         <v>914</v>
       </c>
@@ -21089,7 +21090,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="403" spans="1:13">
+    <row r="403" spans="1:13" hidden="1">
       <c r="A403" t="s">
         <v>914</v>
       </c>
@@ -21131,7 +21132,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="404" spans="1:13">
+    <row r="404" spans="1:13" hidden="1">
       <c r="A404" t="s">
         <v>914</v>
       </c>
@@ -21173,7 +21174,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="405" spans="1:13">
+    <row r="405" spans="1:13" hidden="1">
       <c r="A405" t="s">
         <v>921</v>
       </c>
@@ -21215,7 +21216,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="406" spans="1:13">
+    <row r="406" spans="1:13" hidden="1">
       <c r="A406" t="s">
         <v>921</v>
       </c>
@@ -21257,7 +21258,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="407" spans="1:13" ht="60">
+    <row r="407" spans="1:13" ht="60" hidden="1">
       <c r="A407" t="s">
         <v>921</v>
       </c>
@@ -21299,7 +21300,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="408" spans="1:13">
+    <row r="408" spans="1:13" hidden="1">
       <c r="A408" t="s">
         <v>928</v>
       </c>
@@ -21341,7 +21342,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="409" spans="1:13">
+    <row r="409" spans="1:13" hidden="1">
       <c r="A409" t="s">
         <v>928</v>
       </c>
@@ -21383,7 +21384,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="410" spans="1:13" ht="60">
+    <row r="410" spans="1:13" ht="60" hidden="1">
       <c r="A410" t="s">
         <v>928</v>
       </c>
@@ -21425,7 +21426,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="411" spans="1:13">
+    <row r="411" spans="1:13" hidden="1">
       <c r="A411" t="s">
         <v>932</v>
       </c>
@@ -21467,7 +21468,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="412" spans="1:13">
+    <row r="412" spans="1:13" hidden="1">
       <c r="A412" t="s">
         <v>932</v>
       </c>
@@ -21509,7 +21510,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="413" spans="1:13">
+    <row r="413" spans="1:13" hidden="1">
       <c r="A413" t="s">
         <v>932</v>
       </c>
@@ -21551,7 +21552,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="414" spans="1:13">
+    <row r="414" spans="1:13" hidden="1">
       <c r="A414" t="s">
         <v>939</v>
       </c>
@@ -21593,7 +21594,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="415" spans="1:13">
+    <row r="415" spans="1:13" hidden="1">
       <c r="A415" s="4">
         <v>1250</v>
       </c>
@@ -21635,7 +21636,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="416" spans="1:13">
+    <row r="416" spans="1:13" hidden="1">
       <c r="A416" t="s">
         <v>939</v>
       </c>
@@ -21677,7 +21678,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="417" spans="1:13">
+    <row r="417" spans="1:13" hidden="1">
       <c r="A417" t="s">
         <v>945</v>
       </c>
@@ -21719,7 +21720,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="418" spans="1:13">
+    <row r="418" spans="1:13" hidden="1">
       <c r="A418" s="4">
         <v>1253</v>
       </c>
@@ -21761,7 +21762,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="419" spans="1:13">
+    <row r="419" spans="1:13" hidden="1">
       <c r="A419" t="s">
         <v>945</v>
       </c>
@@ -21803,7 +21804,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="420" spans="1:13">
+    <row r="420" spans="1:13" hidden="1">
       <c r="A420" s="4" t="s">
         <v>953</v>
       </c>
@@ -21845,7 +21846,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="421" spans="1:13">
+    <row r="421" spans="1:13" hidden="1">
       <c r="A421" s="4">
         <v>1260</v>
       </c>
@@ -21887,7 +21888,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="422" spans="1:13">
+    <row r="422" spans="1:13" hidden="1">
       <c r="A422" s="4" t="s">
         <v>953</v>
       </c>
@@ -21929,7 +21930,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="423" spans="1:13">
+    <row r="423" spans="1:13" hidden="1">
       <c r="A423" t="s">
         <v>961</v>
       </c>
@@ -21971,7 +21972,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="424" spans="1:13">
+    <row r="424" spans="1:13" hidden="1">
       <c r="A424" t="s">
         <v>966</v>
       </c>
@@ -22013,7 +22014,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="425" spans="1:13">
+    <row r="425" spans="1:13" hidden="1">
       <c r="A425" t="s">
         <v>970</v>
       </c>
@@ -22055,7 +22056,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="426" spans="1:13">
+    <row r="426" spans="1:13" hidden="1">
       <c r="A426" t="s">
         <v>974</v>
       </c>
@@ -22097,7 +22098,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="427" spans="1:13">
+    <row r="427" spans="1:13" hidden="1">
       <c r="A427" t="s">
         <v>978</v>
       </c>
@@ -22139,7 +22140,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="428" spans="1:13">
+    <row r="428" spans="1:13" hidden="1">
       <c r="A428" t="s">
         <v>982</v>
       </c>
@@ -22181,7 +22182,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="429" spans="1:13">
+    <row r="429" spans="1:13" hidden="1">
       <c r="A429" t="s">
         <v>961</v>
       </c>
@@ -22223,7 +22224,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="430" spans="1:13">
+    <row r="430" spans="1:13" hidden="1">
       <c r="A430" t="s">
         <v>966</v>
       </c>
@@ -22265,7 +22266,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="431" spans="1:13">
+    <row r="431" spans="1:13" hidden="1">
       <c r="A431" t="s">
         <v>970</v>
       </c>
@@ -22307,7 +22308,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="432" spans="1:13">
+    <row r="432" spans="1:13" hidden="1">
       <c r="A432" t="s">
         <v>974</v>
       </c>
@@ -22349,7 +22350,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="433" spans="1:13">
+    <row r="433" spans="1:13" hidden="1">
       <c r="A433" t="s">
         <v>978</v>
       </c>
@@ -22391,7 +22392,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="434" spans="1:13">
+    <row r="434" spans="1:13" hidden="1">
       <c r="A434" t="s">
         <v>982</v>
       </c>
@@ -22433,7 +22434,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="435" spans="1:13">
+    <row r="435" spans="1:13" hidden="1">
       <c r="A435" t="s">
         <v>986</v>
       </c>
@@ -22475,7 +22476,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="436" spans="1:13">
+    <row r="436" spans="1:13" hidden="1">
       <c r="A436" s="4">
         <v>1269</v>
       </c>
@@ -22517,7 +22518,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="437" spans="1:13">
+    <row r="437" spans="1:13" hidden="1">
       <c r="A437" t="s">
         <v>986</v>
       </c>
@@ -22559,7 +22560,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="438" spans="1:13" ht="165">
+    <row r="438" spans="1:13" ht="165" hidden="1">
       <c r="A438" t="s">
         <v>995</v>
       </c>
@@ -22601,7 +22602,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="439" spans="1:13" ht="180">
+    <row r="439" spans="1:13" ht="180" hidden="1">
       <c r="A439" t="s">
         <v>995</v>
       </c>
@@ -22643,7 +22644,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="440" spans="1:13" ht="90">
+    <row r="440" spans="1:13" ht="90" hidden="1">
       <c r="A440" t="s">
         <v>995</v>
       </c>
@@ -22685,7 +22686,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="441" spans="1:13">
+    <row r="441" spans="1:13" hidden="1">
       <c r="A441" t="s">
         <v>1003</v>
       </c>
@@ -22724,7 +22725,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="442" spans="1:13" ht="150">
+    <row r="442" spans="1:13" ht="150" hidden="1">
       <c r="A442" t="s">
         <v>1003</v>
       </c>
@@ -22766,7 +22767,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="443" spans="1:13" ht="30">
+    <row r="443" spans="1:13" ht="30" hidden="1">
       <c r="A443" t="s">
         <v>1003</v>
       </c>
@@ -22805,7 +22806,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="444" spans="1:13">
+    <row r="444" spans="1:13" hidden="1">
       <c r="A444" t="s">
         <v>1009</v>
       </c>
@@ -22847,7 +22848,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="445" spans="1:13">
+    <row r="445" spans="1:13" hidden="1">
       <c r="A445" t="s">
         <v>1009</v>
       </c>
@@ -22889,7 +22890,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="446" spans="1:13" ht="30">
+    <row r="446" spans="1:13" ht="30" hidden="1">
       <c r="A446" t="s">
         <v>1009</v>
       </c>
@@ -22931,7 +22932,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="447" spans="1:13">
+    <row r="447" spans="1:13" hidden="1">
       <c r="A447" t="s">
         <v>1014</v>
       </c>
@@ -22973,7 +22974,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="448" spans="1:13">
+    <row r="448" spans="1:13" hidden="1">
       <c r="A448" t="s">
         <v>1014</v>
       </c>
@@ -23015,7 +23016,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="449" spans="1:13">
+    <row r="449" spans="1:13" hidden="1">
       <c r="A449" t="s">
         <v>1014</v>
       </c>
@@ -23057,7 +23058,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="450" spans="1:13">
+    <row r="450" spans="1:13" hidden="1">
       <c r="A450" t="s">
         <v>1019</v>
       </c>
@@ -23099,7 +23100,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="451" spans="1:13">
+    <row r="451" spans="1:13" hidden="1">
       <c r="A451" t="s">
         <v>1019</v>
       </c>
@@ -23141,7 +23142,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="452" spans="1:13">
+    <row r="452" spans="1:13" hidden="1">
       <c r="A452" t="s">
         <v>1019</v>
       </c>
@@ -23183,7 +23184,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="453" spans="1:13">
+    <row r="453" spans="1:13" hidden="1">
       <c r="A453" t="s">
         <v>1024</v>
       </c>
@@ -23225,7 +23226,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="454" spans="1:13">
+    <row r="454" spans="1:13" hidden="1">
       <c r="A454" t="s">
         <v>1024</v>
       </c>
@@ -23267,7 +23268,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="455" spans="1:13">
+    <row r="455" spans="1:13" hidden="1">
       <c r="A455" t="s">
         <v>1024</v>
       </c>
@@ -23309,7 +23310,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="456" spans="1:13">
+    <row r="456" spans="1:13" hidden="1">
       <c r="A456" t="s">
         <v>1029</v>
       </c>
@@ -23351,7 +23352,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="457" spans="1:13">
+    <row r="457" spans="1:13" hidden="1">
       <c r="A457" t="s">
         <v>1029</v>
       </c>
@@ -23393,7 +23394,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="458" spans="1:13">
+    <row r="458" spans="1:13" hidden="1">
       <c r="A458" t="s">
         <v>1029</v>
       </c>
@@ -23435,7 +23436,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="459" spans="1:13">
+    <row r="459" spans="1:13" hidden="1">
       <c r="A459" t="s">
         <v>1034</v>
       </c>
@@ -23477,7 +23478,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="460" spans="1:13">
+    <row r="460" spans="1:13" hidden="1">
       <c r="A460" t="s">
         <v>1034</v>
       </c>
@@ -23519,7 +23520,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="461" spans="1:13">
+    <row r="461" spans="1:13" hidden="1">
       <c r="A461" t="s">
         <v>1034</v>
       </c>
@@ -23561,7 +23562,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="462" spans="1:13">
+    <row r="462" spans="1:13" hidden="1">
       <c r="A462" t="s">
         <v>1039</v>
       </c>
@@ -23603,7 +23604,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="463" spans="1:13">
+    <row r="463" spans="1:13" hidden="1">
       <c r="A463" t="s">
         <v>1039</v>
       </c>
@@ -23645,7 +23646,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="464" spans="1:13" ht="30">
+    <row r="464" spans="1:13" ht="30" hidden="1">
       <c r="A464" t="s">
         <v>1039</v>
       </c>
@@ -23688,7 +23689,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:N464"/>
+  <autoFilter ref="A1:N464">
+    <filterColumn colId="9">
+      <filters>
+        <filter val="auth-email-content"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>

</xml_diff>

<commit_message>
corrected template type format table data constraint.
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/template.xlsx
+++ b/mosip_master/xlsx/template.xlsx
@@ -4213,7 +4213,7 @@
   <dimension ref="A1:M464"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D94" sqref="D94"/>
+      <selection activeCell="D64" sqref="D64:D65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15"/>
@@ -4316,7 +4316,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:13" hidden="1">
+    <row r="3" spans="1:13">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -4358,7 +4358,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:13" hidden="1">
+    <row r="4" spans="1:13">
       <c r="A4" t="s">
         <v>27</v>
       </c>
@@ -4400,7 +4400,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:13" hidden="1">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -4526,7 +4526,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="45">
+    <row r="8" spans="1:13" ht="45" hidden="1">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -4649,7 +4649,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:13" hidden="1">
+    <row r="11" spans="1:13">
       <c r="A11" t="s">
         <v>47</v>
       </c>
@@ -4691,7 +4691,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:13" hidden="1">
+    <row r="12" spans="1:13">
       <c r="A12" t="s">
         <v>52</v>
       </c>
@@ -4733,7 +4733,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:13" hidden="1">
+    <row r="13" spans="1:13">
       <c r="A13" t="s">
         <v>56</v>
       </c>
@@ -4775,7 +4775,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:13" hidden="1">
+    <row r="14" spans="1:13">
       <c r="A14" t="s">
         <v>60</v>
       </c>
@@ -4817,7 +4817,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:13" hidden="1">
+    <row r="15" spans="1:13">
       <c r="A15" t="s">
         <v>64</v>
       </c>
@@ -4859,7 +4859,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:13" hidden="1">
+    <row r="16" spans="1:13">
       <c r="A16" t="s">
         <v>68</v>
       </c>
@@ -4901,7 +4901,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:13" hidden="1">
+    <row r="17" spans="1:13">
       <c r="A17" t="s">
         <v>72</v>
       </c>
@@ -4943,7 +4943,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:13" hidden="1">
+    <row r="18" spans="1:13">
       <c r="A18" t="s">
         <v>76</v>
       </c>
@@ -5649,7 +5649,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="35" spans="1:13" hidden="1">
+    <row r="35" spans="1:13">
       <c r="A35" t="s">
         <v>114</v>
       </c>
@@ -5691,7 +5691,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="36" spans="1:13" hidden="1">
+    <row r="36" spans="1:13">
       <c r="A36" t="s">
         <v>119</v>
       </c>
@@ -5733,7 +5733,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="37" spans="1:13" hidden="1">
+    <row r="37" spans="1:13">
       <c r="A37" t="s">
         <v>123</v>
       </c>
@@ -5775,7 +5775,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="38" spans="1:13" hidden="1">
+    <row r="38" spans="1:13">
       <c r="A38" t="s">
         <v>126</v>
       </c>
@@ -5817,7 +5817,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="39" spans="1:13" hidden="1">
+    <row r="39" spans="1:13">
       <c r="A39" t="s">
         <v>130</v>
       </c>
@@ -5859,7 +5859,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="40" spans="1:13" hidden="1">
+    <row r="40" spans="1:13">
       <c r="A40" t="s">
         <v>134</v>
       </c>
@@ -5901,7 +5901,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="41" spans="1:13" hidden="1">
+    <row r="41" spans="1:13">
       <c r="A41" t="s">
         <v>137</v>
       </c>
@@ -5943,7 +5943,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="42" spans="1:13" hidden="1">
+    <row r="42" spans="1:13">
       <c r="A42" t="s">
         <v>141</v>
       </c>
@@ -5985,7 +5985,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="43" spans="1:13" hidden="1">
+    <row r="43" spans="1:13">
       <c r="A43" t="s">
         <v>145</v>
       </c>
@@ -6774,7 +6774,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="62" spans="1:13" hidden="1">
+    <row r="62" spans="1:13">
       <c r="A62" t="s">
         <v>181</v>
       </c>
@@ -6816,7 +6816,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="63" spans="1:13" hidden="1">
+    <row r="63" spans="1:13">
       <c r="A63" t="s">
         <v>186</v>
       </c>
@@ -6858,7 +6858,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="64" spans="1:13" hidden="1">
+    <row r="64" spans="1:13">
       <c r="A64" t="s">
         <v>190</v>
       </c>
@@ -6900,7 +6900,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="65" spans="1:13" hidden="1">
+    <row r="65" spans="1:13">
       <c r="A65" t="s">
         <v>194</v>
       </c>
@@ -6942,7 +6942,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="66" spans="1:13" hidden="1">
+    <row r="66" spans="1:13">
       <c r="A66" t="s">
         <v>198</v>
       </c>
@@ -6984,7 +6984,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="67" spans="1:13" hidden="1">
+    <row r="67" spans="1:13">
       <c r="A67" t="s">
         <v>201</v>
       </c>
@@ -7524,7 +7524,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="80" spans="1:13" hidden="1">
+    <row r="80" spans="1:13">
       <c r="A80" t="s">
         <v>229</v>
       </c>
@@ -7650,7 +7650,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="83" spans="1:13" hidden="1">
+    <row r="83" spans="1:13">
       <c r="A83" t="s">
         <v>237</v>
       </c>
@@ -7776,7 +7776,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="86" spans="1:13" hidden="1">
+    <row r="86" spans="1:13">
       <c r="A86" t="s">
         <v>245</v>
       </c>
@@ -7902,7 +7902,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="89" spans="1:13" hidden="1">
+    <row r="89" spans="1:13">
       <c r="A89" t="s">
         <v>251</v>
       </c>
@@ -8028,7 +8028,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="92" spans="1:13" hidden="1">
+    <row r="92" spans="1:13">
       <c r="A92" t="s">
         <v>258</v>
       </c>
@@ -8154,7 +8154,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="95" spans="1:13" hidden="1">
+    <row r="95" spans="1:13">
       <c r="A95" t="s">
         <v>264</v>
       </c>
@@ -8280,7 +8280,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="98" spans="1:13" hidden="1">
+    <row r="98" spans="1:13">
       <c r="A98" t="s">
         <v>271</v>
       </c>
@@ -8406,7 +8406,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="101" spans="1:13" hidden="1">
+    <row r="101" spans="1:13">
       <c r="A101" t="s">
         <v>284</v>
       </c>
@@ -8532,7 +8532,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="104" spans="1:13" hidden="1">
+    <row r="104" spans="1:13">
       <c r="A104" t="s">
         <v>291</v>
       </c>
@@ -8574,7 +8574,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="105" spans="1:13" hidden="1">
+    <row r="105" spans="1:13">
       <c r="A105" t="s">
         <v>295</v>
       </c>
@@ -8616,7 +8616,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="106" spans="1:13" hidden="1">
+    <row r="106" spans="1:13">
       <c r="A106" t="s">
         <v>297</v>
       </c>
@@ -8658,7 +8658,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="107" spans="1:13" hidden="1">
+    <row r="107" spans="1:13">
       <c r="A107" t="s">
         <v>299</v>
       </c>
@@ -8700,7 +8700,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="108" spans="1:13" hidden="1">
+    <row r="108" spans="1:13">
       <c r="A108" t="s">
         <v>300</v>
       </c>
@@ -8826,7 +8826,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="111" spans="1:13" hidden="1">
+    <row r="111" spans="1:13">
       <c r="A111" t="s">
         <v>308</v>
       </c>
@@ -8952,7 +8952,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="114" spans="1:13" hidden="1">
+    <row r="114" spans="1:13">
       <c r="A114" t="s">
         <v>314</v>
       </c>
@@ -9120,7 +9120,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="118" spans="1:13" hidden="1">
+    <row r="118" spans="1:13">
       <c r="A118" t="s">
         <v>316</v>
       </c>
@@ -9246,7 +9246,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="121" spans="1:13" hidden="1">
+    <row r="121" spans="1:13">
       <c r="A121" t="s">
         <v>319</v>
       </c>
@@ -9330,7 +9330,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="123" spans="1:13" hidden="1">
+    <row r="123" spans="1:13">
       <c r="A123" t="s">
         <v>321</v>
       </c>
@@ -9498,7 +9498,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="127" spans="1:13" hidden="1">
+    <row r="127" spans="1:13">
       <c r="A127" t="s">
         <v>322</v>
       </c>
@@ -9624,7 +9624,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="130" spans="1:13" hidden="1">
+    <row r="130" spans="1:13">
       <c r="A130" t="s">
         <v>323</v>
       </c>
@@ -9708,7 +9708,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="132" spans="1:13" hidden="1">
+    <row r="132" spans="1:13">
       <c r="A132" t="s">
         <v>324</v>
       </c>
@@ -9834,7 +9834,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="135" spans="1:13" hidden="1">
+    <row r="135" spans="1:13">
       <c r="A135" t="s">
         <v>325</v>
       </c>
@@ -9960,7 +9960,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="138" spans="1:13" hidden="1">
+    <row r="138" spans="1:13">
       <c r="A138" t="s">
         <v>333</v>
       </c>
@@ -10086,7 +10086,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="141" spans="1:13" hidden="1">
+    <row r="141" spans="1:13">
       <c r="A141" t="s">
         <v>341</v>
       </c>
@@ -10212,7 +10212,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="144" spans="1:13" hidden="1">
+    <row r="144" spans="1:13">
       <c r="A144" t="s">
         <v>349</v>
       </c>
@@ -10338,7 +10338,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="147" spans="1:13" hidden="1">
+    <row r="147" spans="1:13">
       <c r="A147" t="s">
         <v>357</v>
       </c>
@@ -10464,7 +10464,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="150" spans="1:13" hidden="1">
+    <row r="150" spans="1:13">
       <c r="A150" t="s">
         <v>364</v>
       </c>
@@ -10590,7 +10590,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="153" spans="1:13" hidden="1">
+    <row r="153" spans="1:13">
       <c r="A153" t="s">
         <v>367</v>
       </c>
@@ -10716,7 +10716,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="156" spans="1:13" hidden="1">
+    <row r="156" spans="1:13">
       <c r="A156" t="s">
         <v>372</v>
       </c>
@@ -10842,7 +10842,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="159" spans="1:13" hidden="1">
+    <row r="159" spans="1:13">
       <c r="A159" t="s">
         <v>374</v>
       </c>
@@ -10968,7 +10968,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="162" spans="1:13" hidden="1">
+    <row r="162" spans="1:13">
       <c r="A162" t="s">
         <v>382</v>
       </c>
@@ -11094,7 +11094,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="165" spans="1:13" hidden="1">
+    <row r="165" spans="1:13">
       <c r="A165" t="s">
         <v>390</v>
       </c>
@@ -11220,7 +11220,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="168" spans="1:13" hidden="1">
+    <row r="168" spans="1:13">
       <c r="A168" t="s">
         <v>398</v>
       </c>
@@ -11346,7 +11346,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="171" spans="1:13" hidden="1">
+    <row r="171" spans="1:13">
       <c r="A171" t="s">
         <v>405</v>
       </c>
@@ -11472,7 +11472,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="174" spans="1:13" hidden="1">
+    <row r="174" spans="1:13">
       <c r="A174" t="s">
         <v>415</v>
       </c>
@@ -11598,7 +11598,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="177" spans="1:13" hidden="1">
+    <row r="177" spans="1:13">
       <c r="A177" t="s">
         <v>421</v>
       </c>
@@ -11724,7 +11724,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="180" spans="1:13" hidden="1">
+    <row r="180" spans="1:13">
       <c r="A180" t="s">
         <v>429</v>
       </c>
@@ -11850,7 +11850,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="183" spans="1:13" hidden="1">
+    <row r="183" spans="1:13">
       <c r="A183" t="s">
         <v>437</v>
       </c>
@@ -11976,7 +11976,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="186" spans="1:13" hidden="1">
+    <row r="186" spans="1:13">
       <c r="A186" t="s">
         <v>447</v>
       </c>
@@ -12102,7 +12102,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="189" spans="1:13" hidden="1">
+    <row r="189" spans="1:13">
       <c r="A189" t="s">
         <v>452</v>
       </c>
@@ -12228,7 +12228,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="192" spans="1:13" hidden="1">
+    <row r="192" spans="1:13">
       <c r="A192" t="s">
         <v>460</v>
       </c>
@@ -12354,7 +12354,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="195" spans="1:13" hidden="1">
+    <row r="195" spans="1:13">
       <c r="A195" t="s">
         <v>468</v>
       </c>
@@ -12480,7 +12480,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="198" spans="1:13" hidden="1">
+    <row r="198" spans="1:13">
       <c r="A198" t="s">
         <v>473</v>
       </c>
@@ -12606,7 +12606,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="201" spans="1:13" hidden="1">
+    <row r="201" spans="1:13">
       <c r="A201" t="s">
         <v>481</v>
       </c>
@@ -12732,7 +12732,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="204" spans="1:13" hidden="1">
+    <row r="204" spans="1:13">
       <c r="A204" t="s">
         <v>489</v>
       </c>
@@ -12858,7 +12858,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="207" spans="1:13" hidden="1">
+    <row r="207" spans="1:13">
       <c r="A207" t="s">
         <v>494</v>
       </c>
@@ -12984,7 +12984,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="210" spans="1:13" hidden="1">
+    <row r="210" spans="1:13">
       <c r="A210" t="s">
         <v>502</v>
       </c>
@@ -13110,7 +13110,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="213" spans="1:13" hidden="1">
+    <row r="213" spans="1:13">
       <c r="A213" t="s">
         <v>510</v>
       </c>
@@ -13236,7 +13236,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="216" spans="1:13" hidden="1">
+    <row r="216" spans="1:13">
       <c r="A216" t="s">
         <v>515</v>
       </c>
@@ -13362,7 +13362,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="219" spans="1:13" hidden="1">
+    <row r="219" spans="1:13">
       <c r="A219" t="s">
         <v>523</v>
       </c>
@@ -13488,7 +13488,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="222" spans="1:13" hidden="1">
+    <row r="222" spans="1:13">
       <c r="A222" t="s">
         <v>531</v>
       </c>
@@ -13614,7 +13614,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="225" spans="1:13" hidden="1">
+    <row r="225" spans="1:13">
       <c r="A225" t="s">
         <v>536</v>
       </c>
@@ -13740,7 +13740,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="228" spans="1:13" hidden="1">
+    <row r="228" spans="1:13">
       <c r="A228" t="s">
         <v>544</v>
       </c>
@@ -13866,7 +13866,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="231" spans="1:13" hidden="1">
+    <row r="231" spans="1:13">
       <c r="A231" t="s">
         <v>552</v>
       </c>
@@ -13992,7 +13992,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="234" spans="1:13" hidden="1">
+    <row r="234" spans="1:13">
       <c r="A234" t="s">
         <v>557</v>
       </c>
@@ -14118,7 +14118,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="237" spans="1:13" hidden="1">
+    <row r="237" spans="1:13">
       <c r="A237" t="s">
         <v>565</v>
       </c>
@@ -14244,7 +14244,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="240" spans="1:13" hidden="1">
+    <row r="240" spans="1:13">
       <c r="A240" t="s">
         <v>573</v>
       </c>
@@ -14370,7 +14370,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="243" spans="1:13" hidden="1">
+    <row r="243" spans="1:13">
       <c r="A243" t="s">
         <v>580</v>
       </c>
@@ -14496,7 +14496,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="246" spans="1:13" hidden="1">
+    <row r="246" spans="1:13">
       <c r="A246" t="s">
         <v>588</v>
       </c>
@@ -14622,7 +14622,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="249" spans="1:13" hidden="1">
+    <row r="249" spans="1:13">
       <c r="A249" t="s">
         <v>596</v>
       </c>
@@ -14748,7 +14748,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="252" spans="1:13" hidden="1">
+    <row r="252" spans="1:13">
       <c r="A252" t="s">
         <v>601</v>
       </c>
@@ -14874,7 +14874,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="255" spans="1:13" hidden="1">
+    <row r="255" spans="1:13">
       <c r="A255" t="s">
         <v>609</v>
       </c>
@@ -15000,7 +15000,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="258" spans="1:13" hidden="1">
+    <row r="258" spans="1:13">
       <c r="A258" t="s">
         <v>617</v>
       </c>
@@ -15126,7 +15126,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="261" spans="1:13" hidden="1">
+    <row r="261" spans="1:13">
       <c r="A261" t="s">
         <v>622</v>
       </c>
@@ -15252,7 +15252,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="264" spans="1:13" hidden="1">
+    <row r="264" spans="1:13">
       <c r="A264" t="s">
         <v>630</v>
       </c>
@@ -15378,7 +15378,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="267" spans="1:13" hidden="1">
+    <row r="267" spans="1:13">
       <c r="A267" t="s">
         <v>638</v>
       </c>
@@ -15504,7 +15504,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="270" spans="1:13" hidden="1">
+    <row r="270" spans="1:13">
       <c r="A270" t="s">
         <v>643</v>
       </c>
@@ -15630,7 +15630,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="273" spans="1:13" hidden="1">
+    <row r="273" spans="1:13">
       <c r="A273" t="s">
         <v>651</v>
       </c>
@@ -15756,7 +15756,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="276" spans="1:13" hidden="1">
+    <row r="276" spans="1:13">
       <c r="A276" t="s">
         <v>659</v>
       </c>
@@ -15882,7 +15882,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="279" spans="1:13" hidden="1">
+    <row r="279" spans="1:13">
       <c r="A279" t="s">
         <v>664</v>
       </c>
@@ -16008,7 +16008,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="282" spans="1:13" hidden="1">
+    <row r="282" spans="1:13">
       <c r="A282" t="s">
         <v>672</v>
       </c>
@@ -16134,7 +16134,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="285" spans="1:13" hidden="1">
+    <row r="285" spans="1:13">
       <c r="A285" t="s">
         <v>678</v>
       </c>
@@ -16260,7 +16260,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="288" spans="1:13" hidden="1">
+    <row r="288" spans="1:13">
       <c r="A288" t="s">
         <v>683</v>
       </c>
@@ -16386,7 +16386,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="291" spans="1:13" hidden="1">
+    <row r="291" spans="1:13">
       <c r="A291" t="s">
         <v>691</v>
       </c>
@@ -16512,7 +16512,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="294" spans="1:13" hidden="1">
+    <row r="294" spans="1:13">
       <c r="A294" t="s">
         <v>699</v>
       </c>
@@ -16638,7 +16638,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="297" spans="1:13" hidden="1">
+    <row r="297" spans="1:13">
       <c r="A297" t="s">
         <v>704</v>
       </c>
@@ -16764,7 +16764,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="300" spans="1:13" hidden="1">
+    <row r="300" spans="1:13">
       <c r="A300" t="s">
         <v>712</v>
       </c>
@@ -16890,7 +16890,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="303" spans="1:13" hidden="1">
+    <row r="303" spans="1:13">
       <c r="A303" t="s">
         <v>720</v>
       </c>
@@ -17016,7 +17016,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="306" spans="1:13" hidden="1">
+    <row r="306" spans="1:13">
       <c r="A306" t="s">
         <v>725</v>
       </c>
@@ -17142,7 +17142,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="309" spans="1:13" hidden="1">
+    <row r="309" spans="1:13">
       <c r="A309" t="s">
         <v>733</v>
       </c>
@@ -17268,7 +17268,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="312" spans="1:13" hidden="1">
+    <row r="312" spans="1:13">
       <c r="A312" t="s">
         <v>741</v>
       </c>
@@ -17394,7 +17394,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="315" spans="1:13" hidden="1">
+    <row r="315" spans="1:13">
       <c r="A315" t="s">
         <v>746</v>
       </c>
@@ -17520,7 +17520,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="318" spans="1:13" hidden="1">
+    <row r="318" spans="1:13">
       <c r="A318" t="s">
         <v>753</v>
       </c>
@@ -17646,7 +17646,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="321" spans="1:13" hidden="1">
+    <row r="321" spans="1:13">
       <c r="A321" t="s">
         <v>757</v>
       </c>
@@ -17772,7 +17772,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="324" spans="1:13" hidden="1">
+    <row r="324" spans="1:13">
       <c r="A324" t="s">
         <v>764</v>
       </c>
@@ -17898,7 +17898,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="327" spans="1:13" hidden="1">
+    <row r="327" spans="1:13">
       <c r="A327" t="s">
         <v>768</v>
       </c>
@@ -18024,7 +18024,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="330" spans="1:13" hidden="1">
+    <row r="330" spans="1:13">
       <c r="A330" t="s">
         <v>775</v>
       </c>
@@ -18150,7 +18150,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="333" spans="1:13" hidden="1">
+    <row r="333" spans="1:13">
       <c r="A333" t="s">
         <v>779</v>
       </c>
@@ -18276,7 +18276,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="336" spans="1:13" hidden="1">
+    <row r="336" spans="1:13">
       <c r="A336" t="s">
         <v>783</v>
       </c>
@@ -18402,7 +18402,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="339" spans="1:13" hidden="1">
+    <row r="339" spans="1:13">
       <c r="A339" t="s">
         <v>787</v>
       </c>
@@ -18528,7 +18528,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="342" spans="1:13" hidden="1">
+    <row r="342" spans="1:13">
       <c r="A342" t="s">
         <v>794</v>
       </c>
@@ -18654,7 +18654,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="345" spans="1:13" hidden="1">
+    <row r="345" spans="1:13">
       <c r="A345" t="s">
         <v>798</v>
       </c>
@@ -18780,7 +18780,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="348" spans="1:13" hidden="1">
+    <row r="348" spans="1:13">
       <c r="A348" t="s">
         <v>805</v>
       </c>
@@ -18906,7 +18906,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="351" spans="1:13" hidden="1">
+    <row r="351" spans="1:13">
       <c r="A351" t="s">
         <v>809</v>
       </c>
@@ -19032,7 +19032,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="354" spans="1:13" hidden="1">
+    <row r="354" spans="1:13">
       <c r="A354" t="s">
         <v>816</v>
       </c>
@@ -19158,7 +19158,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="357" spans="1:13" hidden="1">
+    <row r="357" spans="1:13">
       <c r="A357" t="s">
         <v>820</v>
       </c>
@@ -19284,7 +19284,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="360" spans="1:13" hidden="1">
+    <row r="360" spans="1:13">
       <c r="A360" t="s">
         <v>826</v>
       </c>
@@ -19410,7 +19410,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="363" spans="1:13" hidden="1">
+    <row r="363" spans="1:13">
       <c r="A363" t="s">
         <v>833</v>
       </c>
@@ -19536,7 +19536,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="366" spans="1:13" hidden="1">
+    <row r="366" spans="1:13">
       <c r="A366" t="s">
         <v>840</v>
       </c>
@@ -19662,7 +19662,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="369" spans="1:13" hidden="1">
+    <row r="369" spans="1:13">
       <c r="A369" t="s">
         <v>847</v>
       </c>
@@ -19788,7 +19788,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="372" spans="1:13" hidden="1">
+    <row r="372" spans="1:13">
       <c r="A372" t="s">
         <v>851</v>
       </c>
@@ -19914,7 +19914,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="375" spans="1:13" hidden="1">
+    <row r="375" spans="1:13">
       <c r="A375" t="s">
         <v>858</v>
       </c>
@@ -20040,7 +20040,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="378" spans="1:13" hidden="1">
+    <row r="378" spans="1:13">
       <c r="A378" t="s">
         <v>865</v>
       </c>
@@ -20166,7 +20166,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="381" spans="1:13" hidden="1">
+    <row r="381" spans="1:13">
       <c r="A381" t="s">
         <v>872</v>
       </c>
@@ -20292,7 +20292,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="384" spans="1:13" hidden="1">
+    <row r="384" spans="1:13">
       <c r="A384" t="s">
         <v>876</v>
       </c>
@@ -20418,7 +20418,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="387" spans="1:13" hidden="1">
+    <row r="387" spans="1:13">
       <c r="A387" t="s">
         <v>883</v>
       </c>
@@ -20544,7 +20544,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="390" spans="1:13" hidden="1">
+    <row r="390" spans="1:13">
       <c r="A390" t="s">
         <v>890</v>
       </c>
@@ -20670,7 +20670,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="393" spans="1:13" hidden="1">
+    <row r="393" spans="1:13">
       <c r="A393" t="s">
         <v>894</v>
       </c>
@@ -20796,7 +20796,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="396" spans="1:13" hidden="1">
+    <row r="396" spans="1:13">
       <c r="A396" t="s">
         <v>901</v>
       </c>
@@ -20922,7 +20922,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="399" spans="1:13" hidden="1">
+    <row r="399" spans="1:13">
       <c r="A399" t="s">
         <v>908</v>
       </c>
@@ -21048,7 +21048,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="402" spans="1:13" hidden="1">
+    <row r="402" spans="1:13">
       <c r="A402" t="s">
         <v>914</v>
       </c>
@@ -21174,7 +21174,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="405" spans="1:13" hidden="1">
+    <row r="405" spans="1:13">
       <c r="A405" t="s">
         <v>921</v>
       </c>
@@ -21300,7 +21300,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="408" spans="1:13" hidden="1">
+    <row r="408" spans="1:13">
       <c r="A408" t="s">
         <v>928</v>
       </c>
@@ -21426,7 +21426,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="411" spans="1:13" hidden="1">
+    <row r="411" spans="1:13">
       <c r="A411" t="s">
         <v>932</v>
       </c>
@@ -21552,7 +21552,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="414" spans="1:13" hidden="1">
+    <row r="414" spans="1:13">
       <c r="A414" t="s">
         <v>939</v>
       </c>
@@ -21678,7 +21678,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="417" spans="1:13" hidden="1">
+    <row r="417" spans="1:13">
       <c r="A417" t="s">
         <v>945</v>
       </c>
@@ -21804,7 +21804,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="420" spans="1:13" hidden="1">
+    <row r="420" spans="1:13">
       <c r="A420" s="4" t="s">
         <v>953</v>
       </c>
@@ -21930,7 +21930,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="423" spans="1:13" hidden="1">
+    <row r="423" spans="1:13">
       <c r="A423" t="s">
         <v>961</v>
       </c>
@@ -21972,7 +21972,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="424" spans="1:13" hidden="1">
+    <row r="424" spans="1:13">
       <c r="A424" t="s">
         <v>966</v>
       </c>
@@ -22014,7 +22014,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="425" spans="1:13" hidden="1">
+    <row r="425" spans="1:13">
       <c r="A425" t="s">
         <v>970</v>
       </c>
@@ -22056,7 +22056,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="426" spans="1:13" hidden="1">
+    <row r="426" spans="1:13">
       <c r="A426" t="s">
         <v>974</v>
       </c>
@@ -22098,7 +22098,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="427" spans="1:13" hidden="1">
+    <row r="427" spans="1:13">
       <c r="A427" t="s">
         <v>978</v>
       </c>
@@ -22140,7 +22140,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="428" spans="1:13" hidden="1">
+    <row r="428" spans="1:13">
       <c r="A428" t="s">
         <v>982</v>
       </c>
@@ -22434,7 +22434,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="435" spans="1:13" hidden="1">
+    <row r="435" spans="1:13">
       <c r="A435" t="s">
         <v>986</v>
       </c>
@@ -22560,7 +22560,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="438" spans="1:13" ht="165" hidden="1">
+    <row r="438" spans="1:13" ht="165">
       <c r="A438" t="s">
         <v>995</v>
       </c>
@@ -22686,7 +22686,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="441" spans="1:13" hidden="1">
+    <row r="441" spans="1:13">
       <c r="A441" t="s">
         <v>1003</v>
       </c>
@@ -22806,7 +22806,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="444" spans="1:13" hidden="1">
+    <row r="444" spans="1:13">
       <c r="A444" t="s">
         <v>1009</v>
       </c>
@@ -22932,7 +22932,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="447" spans="1:13" hidden="1">
+    <row r="447" spans="1:13">
       <c r="A447" t="s">
         <v>1014</v>
       </c>
@@ -23058,7 +23058,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="450" spans="1:13" hidden="1">
+    <row r="450" spans="1:13">
       <c r="A450" t="s">
         <v>1019</v>
       </c>
@@ -23184,7 +23184,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="453" spans="1:13" hidden="1">
+    <row r="453" spans="1:13">
       <c r="A453" t="s">
         <v>1024</v>
       </c>
@@ -23310,7 +23310,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="456" spans="1:13" hidden="1">
+    <row r="456" spans="1:13">
       <c r="A456" t="s">
         <v>1029</v>
       </c>
@@ -23436,7 +23436,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="459" spans="1:13" hidden="1">
+    <row r="459" spans="1:13">
       <c r="A459" t="s">
         <v>1034</v>
       </c>
@@ -23562,7 +23562,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="462" spans="1:13" hidden="1">
+    <row r="462" spans="1:13">
       <c r="A462" t="s">
         <v>1039</v>
       </c>
@@ -23690,9 +23690,9 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:N464">
-    <filterColumn colId="9">
+    <filterColumn colId="1">
       <filters>
-        <filter val="auth-email-content"/>
+        <filter val="eng"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>

<commit_message>
[MOSIP-18192] Added new Template for Cancel Appointment Email Subject
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/template.xlsx
+++ b/mosip_master/xlsx/template.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Develop_Branch_all\mosip-data\mosip_master\xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\M1072510\Documents\GitHub\mosip-data\mosip_master\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6A4D31F-2DB1-4432-919A-A13CBAF177FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" tabRatio="500"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,8 +18,18 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$N$464</definedName>
   </definedNames>
-  <calcPr calcId="162913" iterateDelta="1E-4"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
@@ -27,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5100" uniqueCount="1063">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5130" uniqueCount="1070">
   <si>
     <t>id</t>
   </si>
@@ -3818,11 +3829,32 @@
   <si>
     <t>عزيزي الشريك ، يُرجى العثور على الحالة أدناه لـ apikey $ apiKey واسم السياسة $ PolicyName apikey $ حالة apiKey $ apiKeyStatus وتنتهي في السياسة $ apiKeyExpiresOn حالة $ policyName هي $ policyStatus وتنتهي في $ policyExpiresOn</t>
   </si>
+  <si>
+    <t>Template for email subject of cancel Appointment Acknowledgement</t>
+  </si>
+  <si>
+    <t>Acknowledgement-email-cancelAppointment-subject</t>
+  </si>
+  <si>
+    <t>Modèle d'e-mail faisant l'objet d'un accusé de réception d'annulation de rendez-vous</t>
+  </si>
+  <si>
+    <t>نموذج للبريد الإلكتروني موضوع الإقرار بالإلغاء</t>
+  </si>
+  <si>
+    <t>Appointment Cancelled: Pre-Registration $PRID</t>
+  </si>
+  <si>
+    <t>Rendez-vous annulé : Pré-inscription $PRID</t>
+  </si>
+  <si>
+    <t>تم إلغاء الموعد: التسجيل المسبق PRID$</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
@@ -3883,7 +3915,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -3894,6 +3926,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4208,29 +4243,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:M464"/>
+  <dimension ref="A1:M467"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D64" sqref="D64:D65"/>
+    <sheetView tabSelected="1" topLeftCell="C444" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G465" sqref="G465"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="19.5703125" customWidth="1"/>
-    <col min="2" max="2" width="15.5703125" customWidth="1"/>
+    <col min="1" max="1" width="19.54296875" customWidth="1"/>
+    <col min="2" max="2" width="15.54296875" customWidth="1"/>
     <col min="3" max="3" width="33" customWidth="1"/>
-    <col min="4" max="4" width="30.85546875" customWidth="1"/>
-    <col min="5" max="5" width="11.140625" customWidth="1"/>
-    <col min="6" max="6" width="24.85546875" customWidth="1"/>
-    <col min="7" max="7" width="50.140625" customWidth="1"/>
-    <col min="8" max="8" width="14.42578125" customWidth="1"/>
-    <col min="9" max="9" width="32.7109375" customWidth="1"/>
-    <col min="10" max="10" width="30.85546875" customWidth="1"/>
+    <col min="4" max="4" width="30.81640625" customWidth="1"/>
+    <col min="5" max="5" width="11.1796875" customWidth="1"/>
+    <col min="6" max="6" width="24.81640625" customWidth="1"/>
+    <col min="7" max="7" width="50.1796875" customWidth="1"/>
+    <col min="8" max="8" width="14.453125" customWidth="1"/>
+    <col min="9" max="9" width="32.7265625" customWidth="1"/>
+    <col min="10" max="10" width="30.81640625" customWidth="1"/>
     <col min="11" max="11" width="27" customWidth="1"/>
-    <col min="12" max="12" width="23.7109375" customWidth="1"/>
-    <col min="13" max="14" width="22.7109375" customWidth="1"/>
+    <col min="12" max="12" width="23.7265625" customWidth="1"/>
+    <col min="13" max="14" width="22.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
@@ -4526,7 +4561,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="45" hidden="1">
+    <row r="8" spans="1:13" ht="43.5" hidden="1">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -4608,7 +4643,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="45" hidden="1">
+    <row r="10" spans="1:13" ht="29" hidden="1">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -5321,7 +5356,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="27" spans="1:13" ht="45" hidden="1">
+    <row r="27" spans="1:13" ht="43.5" hidden="1">
       <c r="A27" t="s">
         <v>47</v>
       </c>
@@ -5362,7 +5397,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="28" spans="1:13" ht="45" hidden="1">
+    <row r="28" spans="1:13" ht="43.5" hidden="1">
       <c r="A28" t="s">
         <v>52</v>
       </c>
@@ -5403,7 +5438,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="29" spans="1:13" ht="45" hidden="1">
+    <row r="29" spans="1:13" ht="43.5" hidden="1">
       <c r="A29" t="s">
         <v>56</v>
       </c>
@@ -5444,7 +5479,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="30" spans="1:13" ht="45" hidden="1">
+    <row r="30" spans="1:13" ht="43.5" hidden="1">
       <c r="A30" t="s">
         <v>60</v>
       </c>
@@ -5485,7 +5520,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="31" spans="1:13" ht="30" hidden="1">
+    <row r="31" spans="1:13" ht="29" hidden="1">
       <c r="A31" t="s">
         <v>64</v>
       </c>
@@ -5526,7 +5561,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="32" spans="1:13" ht="30" hidden="1">
+    <row r="32" spans="1:13" ht="29" hidden="1">
       <c r="A32" t="s">
         <v>68</v>
       </c>
@@ -5567,7 +5602,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="33" spans="1:13" ht="45" hidden="1">
+    <row r="33" spans="1:13" ht="43.5" hidden="1">
       <c r="A33" t="s">
         <v>72</v>
       </c>
@@ -5608,7 +5643,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="34" spans="1:13" ht="45" hidden="1">
+    <row r="34" spans="1:13" ht="43.5" hidden="1">
       <c r="A34" t="s">
         <v>76</v>
       </c>
@@ -6405,7 +6440,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="53" spans="1:13" ht="60" hidden="1">
+    <row r="53" spans="1:13" ht="58" hidden="1">
       <c r="A53" t="s">
         <v>114</v>
       </c>
@@ -6446,7 +6481,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="54" spans="1:13" ht="30" hidden="1">
+    <row r="54" spans="1:13" ht="29" hidden="1">
       <c r="A54" t="s">
         <v>119</v>
       </c>
@@ -6487,7 +6522,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="55" spans="1:13" ht="60" hidden="1">
+    <row r="55" spans="1:13" ht="58" hidden="1">
       <c r="A55" t="s">
         <v>123</v>
       </c>
@@ -6528,7 +6563,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="56" spans="1:13" ht="45" hidden="1">
+    <row r="56" spans="1:13" ht="43.5" hidden="1">
       <c r="A56" t="s">
         <v>126</v>
       </c>
@@ -6569,7 +6604,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="57" spans="1:13" ht="30" hidden="1">
+    <row r="57" spans="1:13" hidden="1">
       <c r="A57" t="s">
         <v>130</v>
       </c>
@@ -6610,7 +6645,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="58" spans="1:13" ht="45" hidden="1">
+    <row r="58" spans="1:13" ht="43.5" hidden="1">
       <c r="A58" t="s">
         <v>134</v>
       </c>
@@ -6651,7 +6686,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="59" spans="1:13" ht="60" hidden="1">
+    <row r="59" spans="1:13" ht="58" hidden="1">
       <c r="A59" t="s">
         <v>137</v>
       </c>
@@ -6692,7 +6727,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="60" spans="1:13" ht="30" hidden="1">
+    <row r="60" spans="1:13" ht="29" hidden="1">
       <c r="A60" t="s">
         <v>141</v>
       </c>
@@ -6733,7 +6768,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="61" spans="1:13" ht="60" hidden="1">
+    <row r="61" spans="1:13" ht="58" hidden="1">
       <c r="A61" t="s">
         <v>145</v>
       </c>
@@ -7278,7 +7313,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="74" spans="1:13" ht="90" hidden="1">
+    <row r="74" spans="1:13" ht="87" hidden="1">
       <c r="A74" t="s">
         <v>181</v>
       </c>
@@ -7319,7 +7354,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="75" spans="1:13" ht="30" hidden="1">
+    <row r="75" spans="1:13" ht="29" hidden="1">
       <c r="A75" t="s">
         <v>186</v>
       </c>
@@ -7360,7 +7395,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="76" spans="1:13" ht="45" hidden="1">
+    <row r="76" spans="1:13" ht="29" hidden="1">
       <c r="A76" t="s">
         <v>190</v>
       </c>
@@ -7401,7 +7436,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="77" spans="1:13" ht="30" hidden="1">
+    <row r="77" spans="1:13" hidden="1">
       <c r="A77" t="s">
         <v>194</v>
       </c>
@@ -7442,7 +7477,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="78" spans="1:13" ht="30" hidden="1">
+    <row r="78" spans="1:13" ht="29" hidden="1">
       <c r="A78" t="s">
         <v>198</v>
       </c>
@@ -7483,7 +7518,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="79" spans="1:13" ht="60" hidden="1">
+    <row r="79" spans="1:13" ht="58" hidden="1">
       <c r="A79" t="s">
         <v>201</v>
       </c>
@@ -7860,7 +7895,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="88" spans="1:13" ht="30" hidden="1">
+    <row r="88" spans="1:13" ht="29" hidden="1">
       <c r="A88" t="s">
         <v>245</v>
       </c>
@@ -7986,7 +8021,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="91" spans="1:13" ht="30" hidden="1">
+    <row r="91" spans="1:13" ht="29" hidden="1">
       <c r="A91" t="s">
         <v>251</v>
       </c>
@@ -8112,7 +8147,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="94" spans="1:13" ht="30" hidden="1">
+    <row r="94" spans="1:13" ht="29" hidden="1">
       <c r="A94" t="s">
         <v>258</v>
       </c>
@@ -8238,7 +8273,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="97" spans="1:13" ht="30" hidden="1">
+    <row r="97" spans="1:13" ht="29" hidden="1">
       <c r="A97" t="s">
         <v>264</v>
       </c>
@@ -8364,7 +8399,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="100" spans="1:13" ht="150" hidden="1">
+    <row r="100" spans="1:13" ht="130.5" hidden="1">
       <c r="A100" t="s">
         <v>271</v>
       </c>
@@ -8490,7 +8525,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="103" spans="1:13" ht="150" hidden="1">
+    <row r="103" spans="1:13" ht="130.5" hidden="1">
       <c r="A103" t="s">
         <v>284</v>
       </c>
@@ -9918,7 +9953,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="137" spans="1:13" ht="30" hidden="1">
+    <row r="137" spans="1:13" ht="29" hidden="1">
       <c r="A137" t="s">
         <v>325</v>
       </c>
@@ -10170,7 +10205,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="143" spans="1:13" ht="30" hidden="1">
+    <row r="143" spans="1:13" ht="29" hidden="1">
       <c r="A143" t="s">
         <v>341</v>
       </c>
@@ -10296,7 +10331,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="146" spans="1:13" ht="90" hidden="1">
+    <row r="146" spans="1:13" ht="72.5" hidden="1">
       <c r="A146" t="s">
         <v>349</v>
       </c>
@@ -10422,7 +10457,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="149" spans="1:13" ht="30" hidden="1">
+    <row r="149" spans="1:13" ht="29" hidden="1">
       <c r="A149" t="s">
         <v>357</v>
       </c>
@@ -10548,7 +10583,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="152" spans="1:13" ht="30" hidden="1">
+    <row r="152" spans="1:13" ht="29" hidden="1">
       <c r="A152" t="s">
         <v>364</v>
       </c>
@@ -10674,7 +10709,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="155" spans="1:13" ht="45" hidden="1">
+    <row r="155" spans="1:13" ht="29" hidden="1">
       <c r="A155" t="s">
         <v>367</v>
       </c>
@@ -10800,7 +10835,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="158" spans="1:13" ht="45" hidden="1">
+    <row r="158" spans="1:13" ht="29" hidden="1">
       <c r="A158" t="s">
         <v>372</v>
       </c>
@@ -10926,7 +10961,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="161" spans="1:13" ht="60" hidden="1">
+    <row r="161" spans="1:13" ht="58" hidden="1">
       <c r="A161" t="s">
         <v>374</v>
       </c>
@@ -11052,7 +11087,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="164" spans="1:13" ht="45" hidden="1">
+    <row r="164" spans="1:13" ht="29" hidden="1">
       <c r="A164" t="s">
         <v>382</v>
       </c>
@@ -11178,7 +11213,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="167" spans="1:13" ht="45" hidden="1">
+    <row r="167" spans="1:13" ht="43.5" hidden="1">
       <c r="A167" t="s">
         <v>390</v>
       </c>
@@ -11430,7 +11465,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="173" spans="1:13" ht="30" hidden="1">
+    <row r="173" spans="1:13" ht="29" hidden="1">
       <c r="A173" t="s">
         <v>405</v>
       </c>
@@ -11556,7 +11591,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="176" spans="1:13" ht="30" hidden="1">
+    <row r="176" spans="1:13" ht="29" hidden="1">
       <c r="A176" t="s">
         <v>415</v>
       </c>
@@ -11682,7 +11717,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="179" spans="1:13" ht="30" hidden="1">
+    <row r="179" spans="1:13" ht="29" hidden="1">
       <c r="A179" t="s">
         <v>421</v>
       </c>
@@ -11808,7 +11843,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="182" spans="1:13" ht="30" hidden="1">
+    <row r="182" spans="1:13" ht="29" hidden="1">
       <c r="A182" t="s">
         <v>429</v>
       </c>
@@ -11934,7 +11969,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="185" spans="1:13" ht="30" hidden="1">
+    <row r="185" spans="1:13" ht="29" hidden="1">
       <c r="A185" t="s">
         <v>437</v>
       </c>
@@ -12060,7 +12095,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="188" spans="1:13" ht="30" hidden="1">
+    <row r="188" spans="1:13" ht="29" hidden="1">
       <c r="A188" t="s">
         <v>447</v>
       </c>
@@ -12186,7 +12221,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="191" spans="1:13" ht="30" hidden="1">
+    <row r="191" spans="1:13" ht="29" hidden="1">
       <c r="A191" t="s">
         <v>452</v>
       </c>
@@ -12312,7 +12347,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="194" spans="1:13" ht="30" hidden="1">
+    <row r="194" spans="1:13" ht="29" hidden="1">
       <c r="A194" t="s">
         <v>460</v>
       </c>
@@ -12438,7 +12473,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="197" spans="1:13" ht="30" hidden="1">
+    <row r="197" spans="1:13" ht="29" hidden="1">
       <c r="A197" t="s">
         <v>468</v>
       </c>
@@ -12564,7 +12599,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="200" spans="1:13" ht="30" hidden="1">
+    <row r="200" spans="1:13" ht="29" hidden="1">
       <c r="A200" t="s">
         <v>473</v>
       </c>
@@ -12690,7 +12725,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="203" spans="1:13" ht="30" hidden="1">
+    <row r="203" spans="1:13" ht="29" hidden="1">
       <c r="A203" t="s">
         <v>481</v>
       </c>
@@ -12816,7 +12851,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="206" spans="1:13" ht="30" hidden="1">
+    <row r="206" spans="1:13" ht="29" hidden="1">
       <c r="A206" t="s">
         <v>489</v>
       </c>
@@ -12942,7 +12977,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="209" spans="1:13" ht="30" hidden="1">
+    <row r="209" spans="1:13" ht="29" hidden="1">
       <c r="A209" t="s">
         <v>494</v>
       </c>
@@ -13194,7 +13229,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="215" spans="1:13" ht="30" hidden="1">
+    <row r="215" spans="1:13" ht="29" hidden="1">
       <c r="A215" t="s">
         <v>510</v>
       </c>
@@ -13320,7 +13355,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="218" spans="1:13" ht="30" hidden="1">
+    <row r="218" spans="1:13" hidden="1">
       <c r="A218" t="s">
         <v>515</v>
       </c>
@@ -13572,7 +13607,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="224" spans="1:13" ht="30" hidden="1">
+    <row r="224" spans="1:13" hidden="1">
       <c r="A224" t="s">
         <v>531</v>
       </c>
@@ -13698,7 +13733,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="227" spans="1:13" ht="30" hidden="1">
+    <row r="227" spans="1:13" ht="29" hidden="1">
       <c r="A227" t="s">
         <v>536</v>
       </c>
@@ -13950,7 +13985,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="233" spans="1:13" ht="30" hidden="1">
+    <row r="233" spans="1:13" ht="29" hidden="1">
       <c r="A233" t="s">
         <v>552</v>
       </c>
@@ -14076,7 +14111,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="236" spans="1:13" ht="30" hidden="1">
+    <row r="236" spans="1:13" ht="29" hidden="1">
       <c r="A236" t="s">
         <v>557</v>
       </c>
@@ -14202,7 +14237,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="239" spans="1:13" ht="30" hidden="1">
+    <row r="239" spans="1:13" ht="29" hidden="1">
       <c r="A239" t="s">
         <v>565</v>
       </c>
@@ -14328,7 +14363,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="242" spans="1:13" ht="30" hidden="1">
+    <row r="242" spans="1:13" hidden="1">
       <c r="A242" t="s">
         <v>573</v>
       </c>
@@ -14454,7 +14489,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="245" spans="1:13" ht="30" hidden="1">
+    <row r="245" spans="1:13" ht="29" hidden="1">
       <c r="A245" t="s">
         <v>580</v>
       </c>
@@ -14580,7 +14615,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="248" spans="1:13" ht="30" hidden="1">
+    <row r="248" spans="1:13" hidden="1">
       <c r="A248" t="s">
         <v>588</v>
       </c>
@@ -14706,7 +14741,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="251" spans="1:13" ht="30" hidden="1">
+    <row r="251" spans="1:13" ht="29" hidden="1">
       <c r="A251" t="s">
         <v>596</v>
       </c>
@@ -14832,7 +14867,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="254" spans="1:13" ht="30" hidden="1">
+    <row r="254" spans="1:13" ht="29" hidden="1">
       <c r="A254" t="s">
         <v>601</v>
       </c>
@@ -14958,7 +14993,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="257" spans="1:13" ht="30" hidden="1">
+    <row r="257" spans="1:13" ht="29" hidden="1">
       <c r="A257" t="s">
         <v>609</v>
       </c>
@@ -15084,7 +15119,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="260" spans="1:13" ht="30" hidden="1">
+    <row r="260" spans="1:13" ht="29" hidden="1">
       <c r="A260" t="s">
         <v>617</v>
       </c>
@@ -15210,7 +15245,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="263" spans="1:13" ht="30" hidden="1">
+    <row r="263" spans="1:13" ht="29" hidden="1">
       <c r="A263" t="s">
         <v>622</v>
       </c>
@@ -15336,7 +15371,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="266" spans="1:13" ht="30" hidden="1">
+    <row r="266" spans="1:13" ht="29" hidden="1">
       <c r="A266" t="s">
         <v>630</v>
       </c>
@@ -15462,7 +15497,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="269" spans="1:13" ht="30" hidden="1">
+    <row r="269" spans="1:13" ht="29" hidden="1">
       <c r="A269" t="s">
         <v>638</v>
       </c>
@@ -15588,7 +15623,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="272" spans="1:13" ht="30" hidden="1">
+    <row r="272" spans="1:13" ht="29" hidden="1">
       <c r="A272" t="s">
         <v>643</v>
       </c>
@@ -15714,7 +15749,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="275" spans="1:13" ht="30" hidden="1">
+    <row r="275" spans="1:13" ht="29" hidden="1">
       <c r="A275" t="s">
         <v>651</v>
       </c>
@@ -15840,7 +15875,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="278" spans="1:13" ht="30" hidden="1">
+    <row r="278" spans="1:13" ht="29" hidden="1">
       <c r="A278" t="s">
         <v>659</v>
       </c>
@@ -15966,7 +16001,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="281" spans="1:13" ht="30" hidden="1">
+    <row r="281" spans="1:13" ht="29" hidden="1">
       <c r="A281" t="s">
         <v>664</v>
       </c>
@@ -16092,7 +16127,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="284" spans="1:13" ht="30" hidden="1">
+    <row r="284" spans="1:13" ht="29" hidden="1">
       <c r="A284" t="s">
         <v>672</v>
       </c>
@@ -16218,7 +16253,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="287" spans="1:13" ht="30" hidden="1">
+    <row r="287" spans="1:13" ht="29" hidden="1">
       <c r="A287" t="s">
         <v>678</v>
       </c>
@@ -16344,7 +16379,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="290" spans="1:13" ht="30" hidden="1">
+    <row r="290" spans="1:13" ht="29" hidden="1">
       <c r="A290" t="s">
         <v>683</v>
       </c>
@@ -16596,7 +16631,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="296" spans="1:13" ht="30" hidden="1">
+    <row r="296" spans="1:13" ht="29" hidden="1">
       <c r="A296" t="s">
         <v>699</v>
       </c>
@@ -16722,7 +16757,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="299" spans="1:13" ht="30" hidden="1">
+    <row r="299" spans="1:13" ht="29" hidden="1">
       <c r="A299" t="s">
         <v>704</v>
       </c>
@@ -16848,7 +16883,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="302" spans="1:13" ht="30" hidden="1">
+    <row r="302" spans="1:13" ht="29" hidden="1">
       <c r="A302" t="s">
         <v>712</v>
       </c>
@@ -16974,7 +17009,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="305" spans="1:13" ht="30" hidden="1">
+    <row r="305" spans="1:13" ht="29" hidden="1">
       <c r="A305" t="s">
         <v>720</v>
       </c>
@@ -17100,7 +17135,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="308" spans="1:13" ht="30" hidden="1">
+    <row r="308" spans="1:13" ht="29" hidden="1">
       <c r="A308" t="s">
         <v>725</v>
       </c>
@@ -17226,7 +17261,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="311" spans="1:13" ht="30" hidden="1">
+    <row r="311" spans="1:13" ht="29" hidden="1">
       <c r="A311" t="s">
         <v>733</v>
       </c>
@@ -17352,7 +17387,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="314" spans="1:13" ht="30" hidden="1">
+    <row r="314" spans="1:13" ht="29" hidden="1">
       <c r="A314" t="s">
         <v>741</v>
       </c>
@@ -17478,7 +17513,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="317" spans="1:13" ht="30" hidden="1">
+    <row r="317" spans="1:13" ht="29" hidden="1">
       <c r="A317" t="s">
         <v>746</v>
       </c>
@@ -17604,7 +17639,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="320" spans="1:13" ht="30" hidden="1">
+    <row r="320" spans="1:13" ht="29" hidden="1">
       <c r="A320" t="s">
         <v>753</v>
       </c>
@@ -17730,7 +17765,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="323" spans="1:13" ht="30" hidden="1">
+    <row r="323" spans="1:13" ht="29" hidden="1">
       <c r="A323" t="s">
         <v>757</v>
       </c>
@@ -17856,7 +17891,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="326" spans="1:13" ht="30" hidden="1">
+    <row r="326" spans="1:13" ht="29" hidden="1">
       <c r="A326" t="s">
         <v>764</v>
       </c>
@@ -17982,7 +18017,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="329" spans="1:13" ht="30" hidden="1">
+    <row r="329" spans="1:13" ht="29" hidden="1">
       <c r="A329" t="s">
         <v>768</v>
       </c>
@@ -18108,7 +18143,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="332" spans="1:13" ht="30" hidden="1">
+    <row r="332" spans="1:13" ht="29" hidden="1">
       <c r="A332" t="s">
         <v>775</v>
       </c>
@@ -18234,7 +18269,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="335" spans="1:13" ht="30" hidden="1">
+    <row r="335" spans="1:13" ht="29" hidden="1">
       <c r="A335" t="s">
         <v>779</v>
       </c>
@@ -18360,7 +18395,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="338" spans="1:13" ht="30" hidden="1">
+    <row r="338" spans="1:13" ht="29" hidden="1">
       <c r="A338" t="s">
         <v>783</v>
       </c>
@@ -18486,7 +18521,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="341" spans="1:13" ht="30" hidden="1">
+    <row r="341" spans="1:13" ht="29" hidden="1">
       <c r="A341" t="s">
         <v>787</v>
       </c>
@@ -18612,7 +18647,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="344" spans="1:13" ht="30" hidden="1">
+    <row r="344" spans="1:13" ht="29" hidden="1">
       <c r="A344" t="s">
         <v>794</v>
       </c>
@@ -18738,7 +18773,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="347" spans="1:13" ht="30" hidden="1">
+    <row r="347" spans="1:13" ht="29" hidden="1">
       <c r="A347" t="s">
         <v>798</v>
       </c>
@@ -18864,7 +18899,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="350" spans="1:13" ht="30" hidden="1">
+    <row r="350" spans="1:13" ht="29" hidden="1">
       <c r="A350" t="s">
         <v>805</v>
       </c>
@@ -18990,7 +19025,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="353" spans="1:13" ht="30" hidden="1">
+    <row r="353" spans="1:13" ht="29" hidden="1">
       <c r="A353" t="s">
         <v>809</v>
       </c>
@@ -19116,7 +19151,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="356" spans="1:13" ht="30" hidden="1">
+    <row r="356" spans="1:13" ht="29" hidden="1">
       <c r="A356" t="s">
         <v>816</v>
       </c>
@@ -19242,7 +19277,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="359" spans="1:13" ht="30" hidden="1">
+    <row r="359" spans="1:13" ht="29" hidden="1">
       <c r="A359" t="s">
         <v>820</v>
       </c>
@@ -19368,7 +19403,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="362" spans="1:13" ht="30" hidden="1">
+    <row r="362" spans="1:13" ht="29" hidden="1">
       <c r="A362" t="s">
         <v>826</v>
       </c>
@@ -19494,7 +19529,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="365" spans="1:13" ht="30" hidden="1">
+    <row r="365" spans="1:13" ht="29" hidden="1">
       <c r="A365" t="s">
         <v>833</v>
       </c>
@@ -19620,7 +19655,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="368" spans="1:13" ht="30" hidden="1">
+    <row r="368" spans="1:13" ht="29" hidden="1">
       <c r="A368" t="s">
         <v>840</v>
       </c>
@@ -19746,7 +19781,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="371" spans="1:13" ht="30" hidden="1">
+    <row r="371" spans="1:13" ht="29" hidden="1">
       <c r="A371" t="s">
         <v>847</v>
       </c>
@@ -19872,7 +19907,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="374" spans="1:13" ht="30" hidden="1">
+    <row r="374" spans="1:13" ht="29" hidden="1">
       <c r="A374" t="s">
         <v>851</v>
       </c>
@@ -19998,7 +20033,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="377" spans="1:13" ht="30" hidden="1">
+    <row r="377" spans="1:13" ht="29" hidden="1">
       <c r="A377" t="s">
         <v>858</v>
       </c>
@@ -20124,7 +20159,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="380" spans="1:13" ht="60" hidden="1">
+    <row r="380" spans="1:13" ht="43.5" hidden="1">
       <c r="A380" t="s">
         <v>865</v>
       </c>
@@ -20250,7 +20285,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="383" spans="1:13" ht="60" hidden="1">
+    <row r="383" spans="1:13" ht="43.5" hidden="1">
       <c r="A383" t="s">
         <v>872</v>
       </c>
@@ -20376,7 +20411,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="386" spans="1:13" ht="30" hidden="1">
+    <row r="386" spans="1:13" hidden="1">
       <c r="A386" t="s">
         <v>876</v>
       </c>
@@ -20502,7 +20537,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="389" spans="1:13" ht="30" hidden="1">
+    <row r="389" spans="1:13" ht="29" hidden="1">
       <c r="A389" t="s">
         <v>883</v>
       </c>
@@ -20628,7 +20663,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="392" spans="1:13" ht="30" hidden="1">
+    <row r="392" spans="1:13" ht="29" hidden="1">
       <c r="A392" t="s">
         <v>890</v>
       </c>
@@ -20754,7 +20789,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="395" spans="1:13" ht="30" hidden="1">
+    <row r="395" spans="1:13" ht="29" hidden="1">
       <c r="A395" t="s">
         <v>894</v>
       </c>
@@ -20880,7 +20915,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="398" spans="1:13" ht="30" hidden="1">
+    <row r="398" spans="1:13" ht="29" hidden="1">
       <c r="A398" t="s">
         <v>901</v>
       </c>
@@ -21006,7 +21041,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="401" spans="1:13" ht="30" hidden="1">
+    <row r="401" spans="1:13" ht="29" hidden="1">
       <c r="A401" t="s">
         <v>908</v>
       </c>
@@ -21258,7 +21293,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="407" spans="1:13" ht="60" hidden="1">
+    <row r="407" spans="1:13" ht="43.5" hidden="1">
       <c r="A407" t="s">
         <v>921</v>
       </c>
@@ -21384,7 +21419,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="410" spans="1:13" ht="60" hidden="1">
+    <row r="410" spans="1:13" ht="43.5" hidden="1">
       <c r="A410" t="s">
         <v>928</v>
       </c>
@@ -22560,7 +22595,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="438" spans="1:13" ht="165">
+    <row r="438" spans="1:13" ht="159.5">
       <c r="A438" t="s">
         <v>995</v>
       </c>
@@ -22602,7 +22637,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="439" spans="1:13" ht="180" hidden="1">
+    <row r="439" spans="1:13" ht="174" hidden="1">
       <c r="A439" t="s">
         <v>995</v>
       </c>
@@ -22644,7 +22679,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="440" spans="1:13" ht="90" hidden="1">
+    <row r="440" spans="1:13" ht="72.5" hidden="1">
       <c r="A440" t="s">
         <v>995</v>
       </c>
@@ -22725,7 +22760,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="442" spans="1:13" ht="150" hidden="1">
+    <row r="442" spans="1:13" ht="145" hidden="1">
       <c r="A442" t="s">
         <v>1003</v>
       </c>
@@ -22767,7 +22802,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="443" spans="1:13" ht="30" hidden="1">
+    <row r="443" spans="1:13" ht="29" hidden="1">
       <c r="A443" t="s">
         <v>1003</v>
       </c>
@@ -22890,7 +22925,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="446" spans="1:13" ht="30" hidden="1">
+    <row r="446" spans="1:13" hidden="1">
       <c r="A446" t="s">
         <v>1009</v>
       </c>
@@ -23646,7 +23681,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="464" spans="1:13" ht="30" hidden="1">
+    <row r="464" spans="1:13" hidden="1">
       <c r="A464" t="s">
         <v>1039</v>
       </c>
@@ -23688,8 +23723,131 @@
         <v>22</v>
       </c>
     </row>
+    <row r="465" spans="1:13">
+      <c r="A465" s="4">
+        <v>1281</v>
+      </c>
+      <c r="B465" t="s">
+        <v>14</v>
+      </c>
+      <c r="C465" t="s">
+        <v>1063</v>
+      </c>
+      <c r="D465" t="s">
+        <v>1063</v>
+      </c>
+      <c r="E465" t="s">
+        <v>16</v>
+      </c>
+      <c r="F465" t="s">
+        <v>17</v>
+      </c>
+      <c r="G465" t="s">
+        <v>1067</v>
+      </c>
+      <c r="H465">
+        <v>10001</v>
+      </c>
+      <c r="I465" t="s">
+        <v>184</v>
+      </c>
+      <c r="J465" t="s">
+        <v>1064</v>
+      </c>
+      <c r="K465" t="b">
+        <v>1</v>
+      </c>
+      <c r="L465" t="s">
+        <v>21</v>
+      </c>
+      <c r="M465" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="466" spans="1:13">
+      <c r="A466" s="4">
+        <v>1281</v>
+      </c>
+      <c r="B466" t="s">
+        <v>31</v>
+      </c>
+      <c r="C466" t="s">
+        <v>1065</v>
+      </c>
+      <c r="D466" t="s">
+        <v>1065</v>
+      </c>
+      <c r="E466" t="s">
+        <v>16</v>
+      </c>
+      <c r="F466" t="s">
+        <v>17</v>
+      </c>
+      <c r="G466" t="s">
+        <v>1068</v>
+      </c>
+      <c r="H466">
+        <v>10001</v>
+      </c>
+      <c r="I466" t="s">
+        <v>207</v>
+      </c>
+      <c r="J466" t="s">
+        <v>1064</v>
+      </c>
+      <c r="K466" t="b">
+        <v>1</v>
+      </c>
+      <c r="L466" t="s">
+        <v>21</v>
+      </c>
+      <c r="M466" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="467" spans="1:13">
+      <c r="A467" s="4">
+        <v>1281</v>
+      </c>
+      <c r="B467" t="s">
+        <v>39</v>
+      </c>
+      <c r="C467" t="s">
+        <v>1066</v>
+      </c>
+      <c r="D467" s="4" t="s">
+        <v>1066</v>
+      </c>
+      <c r="E467" t="s">
+        <v>16</v>
+      </c>
+      <c r="F467" t="s">
+        <v>17</v>
+      </c>
+      <c r="G467" t="s">
+        <v>1069</v>
+      </c>
+      <c r="H467">
+        <v>10001</v>
+      </c>
+      <c r="I467" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="J467" t="s">
+        <v>1064</v>
+      </c>
+      <c r="K467" t="b">
+        <v>1</v>
+      </c>
+      <c r="L467" t="s">
+        <v>21</v>
+      </c>
+      <c r="M467" t="s">
+        <v>22</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:N464">
+  <autoFilter ref="A1:N464" xr:uid="{00000000-0009-0000-0000-000000000000}">
     <filterColumn colId="1">
       <filters>
         <filter val="eng"/>

</xml_diff>